<commit_message>
EDA Updates on some Plots
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C2" t="n">
-        <v>514.0951969813251</v>
+        <v>552.2850352784722</v>
       </c>
       <c r="D2" t="n">
-        <v>115.5876343105687</v>
+        <v>122.486354368838</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>407</v>
       </c>
       <c r="F2" t="n">
-        <v>439</v>
+        <v>469</v>
       </c>
       <c r="G2" t="n">
-        <v>472</v>
+        <v>514</v>
       </c>
       <c r="H2" t="n">
-        <v>547</v>
+        <v>590</v>
       </c>
       <c r="I2" t="n">
-        <v>1593</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="3">
@@ -513,25 +513,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C3" t="n">
-        <v>44.49239140445127</v>
+        <v>45.75903485980964</v>
       </c>
       <c r="D3" t="n">
-        <v>5.128120987462522</v>
+        <v>4.404573265810024</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>32.43</v>
       </c>
       <c r="F3" t="n">
-        <v>40.61</v>
+        <v>42.41</v>
       </c>
       <c r="G3" t="n">
-        <v>44.3</v>
+        <v>45.66</v>
       </c>
       <c r="H3" t="n">
-        <v>47.87</v>
+        <v>48.89</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -544,28 +544,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C4" t="n">
-        <v>1.124991302123305</v>
+        <v>1.815599734026178</v>
       </c>
       <c r="D4" t="n">
-        <v>1.532834298698804</v>
+        <v>5.98815343961479</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.42</v>
+        <v>0.76</v>
       </c>
       <c r="G4" t="n">
-        <v>0.83</v>
+        <v>1.41</v>
       </c>
       <c r="H4" t="n">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="I4" t="n">
-        <v>90.45999999999999</v>
+        <v>637.71</v>
       </c>
     </row>
     <row r="5">
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C5" t="n">
-        <v>315.6739541442824</v>
+        <v>321.6290285798722</v>
       </c>
       <c r="D5" t="n">
-        <v>9.529090836634277</v>
+        <v>3.794901112960051</v>
       </c>
       <c r="E5" t="n">
-        <v>286.91</v>
+        <v>304.31</v>
       </c>
       <c r="F5" t="n">
-        <v>308.5</v>
+        <v>319.24</v>
       </c>
       <c r="G5" t="n">
-        <v>316.86</v>
+        <v>321.56</v>
       </c>
       <c r="H5" t="n">
-        <v>323.59</v>
+        <v>324.74</v>
       </c>
       <c r="I5" t="n">
-        <v>334.37</v>
+        <v>330.38</v>
       </c>
     </row>
     <row r="6">
@@ -606,28 +606,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C6" t="n">
-        <v>22.46868431823996</v>
+        <v>22.21511814901922</v>
       </c>
       <c r="D6" t="n">
-        <v>2.00322478833991</v>
+        <v>1.70474918211924</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>16.2</v>
       </c>
       <c r="F6" t="n">
-        <v>21.35</v>
+        <v>21.29</v>
       </c>
       <c r="G6" t="n">
-        <v>22.21</v>
+        <v>21.84</v>
       </c>
       <c r="H6" t="n">
-        <v>23.64</v>
+        <v>22.74</v>
       </c>
       <c r="I6" t="n">
-        <v>33.01</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="7">
@@ -637,25 +637,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C7" t="n">
-        <v>-77.34233819391149</v>
+        <v>-76.28842151925232</v>
       </c>
       <c r="D7" t="n">
-        <v>23.41110719059232</v>
+        <v>24.07634987098373</v>
       </c>
       <c r="E7" t="n">
-        <v>-123</v>
+        <v>-122</v>
       </c>
       <c r="F7" t="n">
-        <v>-94</v>
+        <v>-96</v>
       </c>
       <c r="G7" t="n">
-        <v>-77</v>
+        <v>-72</v>
       </c>
       <c r="H7" t="n">
-        <v>-54</v>
+        <v>-56</v>
       </c>
       <c r="I7" t="n">
         <v>-32</v>
@@ -668,19 +668,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>156013</v>
+        <v>81089</v>
       </c>
       <c r="C8" t="n">
-        <v>7.714834020241902</v>
+        <v>7.533825796347224</v>
       </c>
       <c r="D8" t="n">
-        <v>6.533607361137567</v>
+        <v>6.592628138518452</v>
       </c>
       <c r="E8" t="n">
-        <v>-24.5</v>
+        <v>-23.8</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="G8" t="n">
         <v>9.5</v>
@@ -689,7 +689,7 @@
         <v>11.2</v>
       </c>
       <c r="I8" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C9" t="n">
-        <v>9.322460987464824</v>
+        <v>9.327640344288335</v>
       </c>
       <c r="D9" t="n">
-        <v>1.689399274803902</v>
+        <v>1.685565108282402</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8296635968278</v>
+        <v>867.8316151752841</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4613697335115277</v>
+        <v>0.4604519342066086</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,28 +761,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C11" t="n">
-        <v>12287.41061013047</v>
+        <v>26773.71921291451</v>
       </c>
       <c r="D11" t="n">
-        <v>7730.967440721413</v>
+        <v>4334.889041327159</v>
       </c>
       <c r="E11" t="n">
-        <v>76</v>
+        <v>18017</v>
       </c>
       <c r="F11" t="n">
-        <v>5409</v>
+        <v>23613.5</v>
       </c>
       <c r="G11" t="n">
-        <v>11906.5</v>
+        <v>26795</v>
       </c>
       <c r="H11" t="n">
-        <v>18619</v>
+        <v>30044.5</v>
       </c>
       <c r="I11" t="n">
-        <v>29508</v>
+        <v>36719</v>
       </c>
     </row>
     <row r="12">
@@ -792,28 +792,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C12" t="n">
-        <v>13761.10282680993</v>
+        <v>29901.93253377006</v>
       </c>
       <c r="D12" t="n">
-        <v>8616.597523412509</v>
+        <v>4766.061616018711</v>
       </c>
       <c r="E12" t="n">
-        <v>104</v>
+        <v>20280</v>
       </c>
       <c r="F12" t="n">
-        <v>6097</v>
+        <v>26432</v>
       </c>
       <c r="G12" t="n">
-        <v>13339</v>
+        <v>29924</v>
       </c>
       <c r="H12" t="n">
-        <v>20845.25</v>
+        <v>33504</v>
       </c>
       <c r="I12" t="n">
-        <v>32155</v>
+        <v>40030</v>
       </c>
     </row>
     <row r="13">
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5572035667434125</v>
+        <v>0.5573775832337985</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5910554183855387</v>
+        <v>0.5900888384686347</v>
       </c>
       <c r="E13" t="n">
         <v>0.071936</v>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C14" t="n">
-        <v>23.04748017395753</v>
+        <v>23.91567644777185</v>
       </c>
       <c r="D14" t="n">
-        <v>12.32911785409372</v>
+        <v>13.42217716876898</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
@@ -872,10 +872,10 @@
         <v>25</v>
       </c>
       <c r="H14" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I14" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
@@ -885,13 +885,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C15" t="n">
-        <v>0.673848810437452</v>
+        <v>0.6728398862223098</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7491140369494177</v>
+        <v>0.7484391091290741</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C16" t="n">
-        <v>1.828300076745971</v>
+        <v>1.835391757274261</v>
       </c>
       <c r="D16" t="n">
-        <v>1.668735266864511</v>
+        <v>1.673899526794093</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -947,28 +947,28 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>156360</v>
+        <v>81211</v>
       </c>
       <c r="C17" t="n">
-        <v>94.74233819391154</v>
+        <v>93.68842151925233</v>
       </c>
       <c r="D17" t="n">
-        <v>23.41110719059053</v>
+        <v>24.07634987097837</v>
       </c>
       <c r="E17" t="n">
         <v>49.4</v>
       </c>
       <c r="F17" t="n">
-        <v>71.40000000000001</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>94.40000000000001</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>111.4</v>
+        <v>113.4</v>
       </c>
       <c r="I17" t="n">
-        <v>140.4</v>
+        <v>139.4</v>
       </c>
     </row>
     <row r="18">
@@ -978,25 +978,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>156013</v>
+        <v>81089</v>
       </c>
       <c r="C18" t="n">
-        <v>-86.4866321511565</v>
+        <v>-85.32753334908405</v>
       </c>
       <c r="D18" t="n">
-        <v>21.1451394460242</v>
+        <v>21.726273662449</v>
       </c>
       <c r="E18" t="n">
-        <v>-125.9574620641016</v>
+        <v>-125.3773603942068</v>
       </c>
       <c r="F18" t="n">
-        <v>-103.8707776445072</v>
+        <v>-104.6286946522615</v>
       </c>
       <c r="G18" t="n">
-        <v>-87.69305820175224</v>
+        <v>-83.5149694202523</v>
       </c>
       <c r="H18" t="n">
-        <v>-65.40304509533891</v>
+        <v>-66.7376019773414</v>
       </c>
       <c r="I18" t="n">
         <v>-33.14609373817283</v>
@@ -1009,28 +1009,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>156013</v>
+        <v>81089</v>
       </c>
       <c r="C19" t="n">
-        <v>-78.77179813091459</v>
+        <v>-77.79370755273685</v>
       </c>
       <c r="D19" t="n">
-        <v>25.4159624695924</v>
+        <v>26.14762289951132</v>
       </c>
       <c r="E19" t="n">
         <v>-145.0217119216414</v>
       </c>
       <c r="F19" t="n">
-        <v>-94.49305820175223</v>
+        <v>-96.41392685158225</v>
       </c>
       <c r="G19" t="n">
-        <v>-76.6389203414338</v>
+        <v>-72.41392685158225</v>
       </c>
       <c r="H19" t="n">
-        <v>-54.41392685158225</v>
+        <v>-56.2778545523916</v>
       </c>
       <c r="I19" t="n">
-        <v>-34.5149694202523</v>
+        <v>-33.49305820175223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Cleaning - Isolation Forest in the House
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C2" t="n">
-        <v>552.2850352784722</v>
+        <v>554.1977950713359</v>
       </c>
       <c r="D2" t="n">
-        <v>122.486354368838</v>
+        <v>133.5912396379997</v>
       </c>
       <c r="E2" t="n">
-        <v>407</v>
+        <v>428</v>
       </c>
       <c r="F2" t="n">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="G2" t="n">
-        <v>514</v>
+        <v>528</v>
       </c>
       <c r="H2" t="n">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="I2" t="n">
-        <v>1510</v>
+        <v>21547</v>
       </c>
     </row>
     <row r="3">
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C3" t="n">
-        <v>45.75903485980964</v>
+        <v>46.57148415786548</v>
       </c>
       <c r="D3" t="n">
-        <v>4.404573265810024</v>
+        <v>4.598651801362192</v>
       </c>
       <c r="E3" t="n">
-        <v>32.43</v>
+        <v>33.54</v>
       </c>
       <c r="F3" t="n">
-        <v>42.41</v>
+        <v>43.29</v>
       </c>
       <c r="G3" t="n">
-        <v>45.66</v>
+        <v>47.06</v>
       </c>
       <c r="H3" t="n">
-        <v>48.89</v>
+        <v>50.24</v>
       </c>
       <c r="I3" t="n">
-        <v>60.19</v>
+        <v>156.65</v>
       </c>
     </row>
     <row r="4">
@@ -544,25 +544,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C4" t="n">
-        <v>1.815599734026178</v>
+        <v>1.779784293743438</v>
       </c>
       <c r="D4" t="n">
-        <v>5.98815343961479</v>
+        <v>6.571023565275307</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="G4" t="n">
-        <v>1.41</v>
+        <v>1.42</v>
       </c>
       <c r="H4" t="n">
-        <v>2.25</v>
+        <v>2.27</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C5" t="n">
-        <v>321.6290285798722</v>
+        <v>324.3457488728305</v>
       </c>
       <c r="D5" t="n">
-        <v>3.794901112960051</v>
+        <v>5.795069576299876</v>
       </c>
       <c r="E5" t="n">
-        <v>304.31</v>
+        <v>3.21</v>
       </c>
       <c r="F5" t="n">
-        <v>319.24</v>
+        <v>319.71</v>
       </c>
       <c r="G5" t="n">
-        <v>321.56</v>
+        <v>323.13</v>
       </c>
       <c r="H5" t="n">
-        <v>324.74</v>
+        <v>327.08</v>
       </c>
       <c r="I5" t="n">
-        <v>330.38</v>
+        <v>341.91</v>
       </c>
     </row>
     <row r="6">
@@ -606,28 +606,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C6" t="n">
-        <v>22.21511814901922</v>
+        <v>22.65055107775925</v>
       </c>
       <c r="D6" t="n">
-        <v>1.70474918211924</v>
+        <v>1.860243104778442</v>
       </c>
       <c r="E6" t="n">
-        <v>16.2</v>
+        <v>20.26</v>
       </c>
       <c r="F6" t="n">
-        <v>21.29</v>
+        <v>21.55</v>
       </c>
       <c r="G6" t="n">
-        <v>21.84</v>
+        <v>22.12</v>
       </c>
       <c r="H6" t="n">
-        <v>22.74</v>
+        <v>23.33</v>
       </c>
       <c r="I6" t="n">
-        <v>31.8</v>
+        <v>174.9</v>
       </c>
     </row>
     <row r="7">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C7" t="n">
-        <v>-76.28842151925232</v>
+        <v>-75.59517633253041</v>
       </c>
       <c r="D7" t="n">
-        <v>24.07634987098373</v>
+        <v>24.20918401097775</v>
       </c>
       <c r="E7" t="n">
         <v>-122</v>
       </c>
       <c r="F7" t="n">
-        <v>-96</v>
+        <v>-93</v>
       </c>
       <c r="G7" t="n">
-        <v>-72</v>
+        <v>-70</v>
       </c>
       <c r="H7" t="n">
         <v>-56</v>
       </c>
       <c r="I7" t="n">
-        <v>-32</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="8">
@@ -668,16 +668,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>81089</v>
+        <v>64652</v>
       </c>
       <c r="C8" t="n">
-        <v>7.533825796347224</v>
+        <v>7.556355565179731</v>
       </c>
       <c r="D8" t="n">
-        <v>6.592628138518452</v>
+        <v>6.488444888421669</v>
       </c>
       <c r="E8" t="n">
-        <v>-23.8</v>
+        <v>-23.5</v>
       </c>
       <c r="F8" t="n">
         <v>7.5</v>
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C9" t="n">
-        <v>9.327640344288335</v>
+        <v>9.326662960904207</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685565108282402</v>
+        <v>1.685725565541909</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8316151752841</v>
+        <v>867.8327589401518</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4604519342066086</v>
+        <v>0.4604865985964184</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,28 +761,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C11" t="n">
-        <v>26773.71921291451</v>
+        <v>30546.10309739979</v>
       </c>
       <c r="D11" t="n">
-        <v>4334.889041327159</v>
+        <v>3555.215012686406</v>
       </c>
       <c r="E11" t="n">
-        <v>18017</v>
+        <v>24377</v>
       </c>
       <c r="F11" t="n">
-        <v>23613.5</v>
+        <v>27797</v>
       </c>
       <c r="G11" t="n">
-        <v>26795</v>
+        <v>30421</v>
       </c>
       <c r="H11" t="n">
-        <v>30044.5</v>
+        <v>33161</v>
       </c>
       <c r="I11" t="n">
-        <v>36719</v>
+        <v>39332</v>
       </c>
     </row>
     <row r="12">
@@ -792,28 +792,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C12" t="n">
-        <v>29901.93253377006</v>
+        <v>55902.7152121549</v>
       </c>
       <c r="D12" t="n">
-        <v>4766.061616018711</v>
+        <v>5548745.797210963</v>
       </c>
       <c r="E12" t="n">
-        <v>20280</v>
+        <v>27427</v>
       </c>
       <c r="F12" t="n">
-        <v>26432</v>
+        <v>31151</v>
       </c>
       <c r="G12" t="n">
-        <v>29924</v>
+        <v>33996</v>
       </c>
       <c r="H12" t="n">
-        <v>33504</v>
+        <v>37019</v>
       </c>
       <c r="I12" t="n">
-        <v>40030</v>
+        <v>1412121428</v>
       </c>
     </row>
     <row r="13">
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5573775832337985</v>
+        <v>0.5571478080415045</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5900888384686347</v>
+        <v>0.5901159743775186</v>
       </c>
       <c r="E13" t="n">
         <v>0.071936</v>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C14" t="n">
-        <v>23.91567644777185</v>
+        <v>23.8592582298808</v>
       </c>
       <c r="D14" t="n">
-        <v>13.42217716876898</v>
+        <v>13.40795884493142</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
@@ -885,13 +885,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6728398862223098</v>
+        <v>0.6710827002655796</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7484391091290741</v>
+        <v>0.7472176997985825</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C16" t="n">
-        <v>1.835391757274261</v>
+        <v>1.829859181026496</v>
       </c>
       <c r="D16" t="n">
-        <v>1.673899526794093</v>
+        <v>1.672220755993723</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -947,25 +947,25 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>81211</v>
+        <v>64764</v>
       </c>
       <c r="C17" t="n">
-        <v>93.68842151925233</v>
+        <v>92.99517633253042</v>
       </c>
       <c r="D17" t="n">
-        <v>24.07634987097837</v>
+        <v>24.20918401097687</v>
       </c>
       <c r="E17" t="n">
-        <v>49.4</v>
+        <v>50.4</v>
       </c>
       <c r="F17" t="n">
         <v>73.40000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>89.40000000000001</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>113.4</v>
+        <v>110.4</v>
       </c>
       <c r="I17" t="n">
         <v>139.4</v>
@@ -978,28 +978,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>81089</v>
+        <v>64652</v>
       </c>
       <c r="C18" t="n">
-        <v>-85.32753334908405</v>
+        <v>-84.61728897300367</v>
       </c>
       <c r="D18" t="n">
-        <v>21.726273662449</v>
+        <v>21.80586520687761</v>
       </c>
       <c r="E18" t="n">
         <v>-125.3773603942068</v>
       </c>
       <c r="F18" t="n">
-        <v>-104.6286946522615</v>
+        <v>-103.1933104806609</v>
       </c>
       <c r="G18" t="n">
-        <v>-83.5149694202523</v>
+        <v>-81.0778545523916</v>
       </c>
       <c r="H18" t="n">
-        <v>-66.7376019773414</v>
+        <v>-66.6389203414338</v>
       </c>
       <c r="I18" t="n">
-        <v>-33.14609373817283</v>
+        <v>-40.37736039420675</v>
       </c>
     </row>
     <row r="19">
@@ -1009,25 +1009,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>81089</v>
+        <v>64652</v>
       </c>
       <c r="C19" t="n">
-        <v>-77.79370755273685</v>
+        <v>-77.06093340782394</v>
       </c>
       <c r="D19" t="n">
-        <v>26.14762289951132</v>
+        <v>26.21709398742338</v>
       </c>
       <c r="E19" t="n">
         <v>-145.0217119216414</v>
       </c>
       <c r="F19" t="n">
-        <v>-96.41392685158225</v>
+        <v>-93.75746206410165</v>
       </c>
       <c r="G19" t="n">
-        <v>-72.41392685158225</v>
+        <v>-70.21238401914255</v>
       </c>
       <c r="H19" t="n">
-        <v>-56.2778545523916</v>
+        <v>-56.34699179957641</v>
       </c>
       <c r="I19" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Data Querry Notebook Advanced to avoid VM overloads + More Data :)
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C2" t="n">
-        <v>554.1977950713359</v>
+        <v>532.9449956670721</v>
       </c>
       <c r="D2" t="n">
-        <v>133.5912396379997</v>
+        <v>113.0475835137304</v>
       </c>
       <c r="E2" t="n">
-        <v>428</v>
+        <v>392</v>
       </c>
       <c r="F2" t="n">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="G2" t="n">
-        <v>528</v>
+        <v>498</v>
       </c>
       <c r="H2" t="n">
-        <v>592</v>
+        <v>577</v>
       </c>
       <c r="I2" t="n">
-        <v>21547</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="3">
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C3" t="n">
-        <v>46.57148415786548</v>
+        <v>44.98589846638205</v>
       </c>
       <c r="D3" t="n">
-        <v>4.598651801362192</v>
+        <v>4.890338910421502</v>
       </c>
       <c r="E3" t="n">
-        <v>33.54</v>
+        <v>30.48</v>
       </c>
       <c r="F3" t="n">
-        <v>43.29</v>
+        <v>41.31</v>
       </c>
       <c r="G3" t="n">
-        <v>47.06</v>
+        <v>44.73</v>
       </c>
       <c r="H3" t="n">
-        <v>50.24</v>
+        <v>48.4</v>
       </c>
       <c r="I3" t="n">
-        <v>156.65</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="4">
@@ -544,25 +544,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C4" t="n">
-        <v>1.779784293743438</v>
+        <v>1.431533816713176</v>
       </c>
       <c r="D4" t="n">
-        <v>6.571023565275307</v>
+        <v>3.591974203725274</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.79</v>
+        <v>0.52</v>
       </c>
       <c r="G4" t="n">
-        <v>1.42</v>
+        <v>1.06</v>
       </c>
       <c r="H4" t="n">
-        <v>2.27</v>
+        <v>1.92</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C5" t="n">
-        <v>324.3457488728305</v>
+        <v>319.7001681096509</v>
       </c>
       <c r="D5" t="n">
-        <v>5.795069576299876</v>
+        <v>9.851875056702589</v>
       </c>
       <c r="E5" t="n">
-        <v>3.21</v>
+        <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>319.71</v>
+        <v>313.79</v>
       </c>
       <c r="G5" t="n">
-        <v>323.13</v>
+        <v>321.37</v>
       </c>
       <c r="H5" t="n">
-        <v>327.08</v>
+        <v>325.75</v>
       </c>
       <c r="I5" t="n">
-        <v>341.91</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6">
@@ -606,28 +606,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C6" t="n">
-        <v>22.65055107775925</v>
+        <v>22.58832927866689</v>
       </c>
       <c r="D6" t="n">
-        <v>1.860243104778442</v>
+        <v>1.9432519255438</v>
       </c>
       <c r="E6" t="n">
-        <v>20.26</v>
+        <v>15.83</v>
       </c>
       <c r="F6" t="n">
-        <v>21.55</v>
+        <v>21.5</v>
       </c>
       <c r="G6" t="n">
-        <v>22.12</v>
+        <v>22.2</v>
       </c>
       <c r="H6" t="n">
-        <v>23.33</v>
+        <v>23.49</v>
       </c>
       <c r="I6" t="n">
-        <v>174.9</v>
+        <v>33.93</v>
       </c>
     </row>
     <row r="7">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C7" t="n">
-        <v>-75.59517633253041</v>
+        <v>-76.56134471820069</v>
       </c>
       <c r="D7" t="n">
-        <v>24.20918401097775</v>
+        <v>23.72077317696776</v>
       </c>
       <c r="E7" t="n">
-        <v>-122</v>
+        <v>-123</v>
       </c>
       <c r="F7" t="n">
-        <v>-93</v>
+        <v>-94</v>
       </c>
       <c r="G7" t="n">
-        <v>-70</v>
+        <v>-74</v>
       </c>
       <c r="H7" t="n">
-        <v>-56</v>
+        <v>-54</v>
       </c>
       <c r="I7" t="n">
-        <v>-33</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="8">
@@ -668,19 +668,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>64652</v>
+        <v>251059</v>
       </c>
       <c r="C8" t="n">
-        <v>7.556355565179731</v>
+        <v>7.671104800066916</v>
       </c>
       <c r="D8" t="n">
-        <v>6.488444888421669</v>
+        <v>6.523565966186341</v>
       </c>
       <c r="E8" t="n">
-        <v>-23.5</v>
+        <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>7.5</v>
+        <v>7.8</v>
       </c>
       <c r="G8" t="n">
         <v>9.5</v>
@@ -689,7 +689,7 @@
         <v>11.2</v>
       </c>
       <c r="I8" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C9" t="n">
-        <v>9.326662960904207</v>
+        <v>9.324361390035062</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685725565541909</v>
+        <v>1.688266393300287</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8327589401518</v>
+        <v>867.8306803094266</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4604865985964184</v>
+        <v>0.4611932605059126</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,28 +761,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>64764</v>
+        <v>251550</v>
       </c>
       <c r="C11" t="n">
-        <v>30546.10309739979</v>
+        <v>17213.86838799443</v>
       </c>
       <c r="D11" t="n">
-        <v>3555.215012686406</v>
+        <v>11936.9850653751</v>
       </c>
       <c r="E11" t="n">
-        <v>24377</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>27797</v>
+        <v>6046.25</v>
       </c>
       <c r="G11" t="n">
-        <v>30421</v>
+        <v>16487.5</v>
       </c>
       <c r="H11" t="n">
-        <v>33161</v>
+        <v>27836</v>
       </c>
       <c r="I11" t="n">
-        <v>39332</v>
+        <v>40744</v>
       </c>
     </row>
     <row r="12">
@@ -792,28 +792,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C12" t="n">
-        <v>55902.7152121549</v>
+        <v>19240.49235973637</v>
       </c>
       <c r="D12" t="n">
-        <v>5548745.797210963</v>
+        <v>13294.66376833996</v>
       </c>
       <c r="E12" t="n">
-        <v>27427</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>31151</v>
+        <v>6817</v>
       </c>
       <c r="G12" t="n">
-        <v>33996</v>
+        <v>18470</v>
       </c>
       <c r="H12" t="n">
-        <v>37019</v>
+        <v>31111</v>
       </c>
       <c r="I12" t="n">
-        <v>1412121428</v>
+        <v>44461</v>
       </c>
     </row>
     <row r="13">
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5571478080415045</v>
+        <v>0.5573166730110272</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5901159743775186</v>
+        <v>0.5906980832801664</v>
       </c>
       <c r="E13" t="n">
         <v>0.071936</v>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C14" t="n">
-        <v>23.8592582298808</v>
+        <v>23.89372798753389</v>
       </c>
       <c r="D14" t="n">
-        <v>13.40795884493142</v>
+        <v>13.4170136097565</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
@@ -885,13 +885,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6710827002655796</v>
+        <v>0.6732614623830309</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7472176997985825</v>
+        <v>0.7487418961972424</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C16" t="n">
-        <v>1.829859181026496</v>
+        <v>1.830041898219922</v>
       </c>
       <c r="D16" t="n">
-        <v>1.672220755993723</v>
+        <v>1.670023765759874</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -947,28 +947,28 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>64764</v>
+        <v>251562</v>
       </c>
       <c r="C17" t="n">
-        <v>92.99517633253042</v>
+        <v>93.96134471820075</v>
       </c>
       <c r="D17" t="n">
-        <v>24.20918401097687</v>
+        <v>23.72077317695606</v>
       </c>
       <c r="E17" t="n">
-        <v>50.4</v>
+        <v>49.4</v>
       </c>
       <c r="F17" t="n">
-        <v>73.40000000000001</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>87.40000000000001</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>110.4</v>
+        <v>111.4</v>
       </c>
       <c r="I17" t="n">
-        <v>139.4</v>
+        <v>140.4</v>
       </c>
     </row>
     <row r="18">
@@ -978,28 +978,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>64652</v>
+        <v>251059</v>
       </c>
       <c r="C18" t="n">
-        <v>-84.61728897300367</v>
+        <v>-85.67615448186591</v>
       </c>
       <c r="D18" t="n">
-        <v>21.80586520687761</v>
+        <v>21.4250801593023</v>
       </c>
       <c r="E18" t="n">
-        <v>-125.3773603942068</v>
+        <v>-125.9574620641016</v>
       </c>
       <c r="F18" t="n">
-        <v>-103.1933104806609</v>
+        <v>-103.3377954106368</v>
       </c>
       <c r="G18" t="n">
-        <v>-81.0778545523916</v>
+        <v>-85.26572375596102</v>
       </c>
       <c r="H18" t="n">
-        <v>-66.6389203414338</v>
+        <v>-65.14699179957641</v>
       </c>
       <c r="I18" t="n">
-        <v>-40.37736039420675</v>
+        <v>-33.14609373817283</v>
       </c>
     </row>
     <row r="19">
@@ -1009,25 +1009,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>64652</v>
+        <v>251059</v>
       </c>
       <c r="C19" t="n">
-        <v>-77.06093340782394</v>
+        <v>-78.00504968179897</v>
       </c>
       <c r="D19" t="n">
-        <v>26.21709398742338</v>
+        <v>25.73412961331832</v>
       </c>
       <c r="E19" t="n">
         <v>-145.0217119216414</v>
       </c>
       <c r="F19" t="n">
-        <v>-93.75746206410165</v>
+        <v>-94.26572375596102</v>
       </c>
       <c r="G19" t="n">
-        <v>-70.21238401914255</v>
+        <v>-74.39612087980606</v>
       </c>
       <c r="H19" t="n">
-        <v>-56.34699179957641</v>
+        <v>-54.34699179957641</v>
       </c>
       <c r="I19" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Modelling - Standard Deviation included, Arrangement of Files updated
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,25 +482,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C2" t="n">
-        <v>530.9836165029951</v>
+        <v>534.0941587234468</v>
       </c>
       <c r="D2" t="n">
-        <v>115.3403164598751</v>
+        <v>116.5276101818023</v>
       </c>
       <c r="E2" t="n">
         <v>390</v>
       </c>
       <c r="F2" t="n">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="H2" t="n">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -513,25 +513,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C3" t="n">
-        <v>45.08549446172229</v>
+        <v>44.90025967428392</v>
       </c>
       <c r="D3" t="n">
-        <v>4.62753711847431</v>
+        <v>4.62925788268382</v>
       </c>
       <c r="E3" t="n">
         <v>30.48</v>
       </c>
       <c r="F3" t="n">
-        <v>41.88</v>
+        <v>41.45</v>
       </c>
       <c r="G3" t="n">
-        <v>45.07</v>
+        <v>44.84</v>
       </c>
       <c r="H3" t="n">
-        <v>48.27</v>
+        <v>48.12</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -544,25 +544,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C4" t="n">
-        <v>1.658366889831936</v>
+        <v>1.705674747901874</v>
       </c>
       <c r="D4" t="n">
-        <v>3.281811852958463</v>
+        <v>3.238081598277234</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="G4" t="n">
-        <v>1.28</v>
+        <v>1.33</v>
       </c>
       <c r="H4" t="n">
-        <v>2.25</v>
+        <v>2.33</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -575,25 +575,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C5" t="n">
-        <v>322.1470204525608</v>
+        <v>322.5149398312103</v>
       </c>
       <c r="D5" t="n">
-        <v>9.90437378467978</v>
+        <v>9.867247193481946</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.56</v>
+        <v>318.08</v>
       </c>
       <c r="G5" t="n">
-        <v>324.01</v>
+        <v>324.39</v>
       </c>
       <c r="H5" t="n">
-        <v>329.53</v>
+        <v>329.84</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -606,25 +606,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C6" t="n">
-        <v>22.54798385243516</v>
+        <v>22.51477858825049</v>
       </c>
       <c r="D6" t="n">
-        <v>1.853291742097564</v>
+        <v>1.835523249557064</v>
       </c>
       <c r="E6" t="n">
         <v>15.83</v>
       </c>
       <c r="F6" t="n">
-        <v>21.55</v>
+        <v>21.52</v>
       </c>
       <c r="G6" t="n">
-        <v>22.22</v>
+        <v>22.19</v>
       </c>
       <c r="H6" t="n">
-        <v>23.21</v>
+        <v>23.13</v>
       </c>
       <c r="I6" t="n">
         <v>34.01</v>
@@ -637,13 +637,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C7" t="n">
-        <v>-76.30858701147488</v>
+        <v>-76.33234079790452</v>
       </c>
       <c r="D7" t="n">
-        <v>23.56389603212708</v>
+        <v>23.56758322221495</v>
       </c>
       <c r="E7" t="n">
         <v>-123</v>
@@ -668,13 +668,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>325815</v>
+        <v>339939</v>
       </c>
       <c r="C8" t="n">
-        <v>7.724178137900343</v>
+        <v>7.720823147682379</v>
       </c>
       <c r="D8" t="n">
-        <v>6.571712309012434</v>
+        <v>6.579145716284592</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C9" t="n">
-        <v>9.324694743615277</v>
+        <v>9.324559085222969</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688232436684749</v>
+        <v>1.688312520378005</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8304398449588</v>
+        <v>867.8304931550293</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461278146729259</v>
+        <v>0.4611783823689606</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,25 +761,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>326353</v>
+        <v>340530</v>
       </c>
       <c r="C11" t="n">
-        <v>15148.88637456987</v>
+        <v>15176.54487416674</v>
       </c>
       <c r="D11" t="n">
-        <v>11289.31142974376</v>
+        <v>11053.5498440258</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>5440</v>
+        <v>5787</v>
       </c>
       <c r="G11" t="n">
-        <v>12442</v>
+        <v>13032</v>
       </c>
       <c r="H11" t="n">
-        <v>24992</v>
+        <v>24291</v>
       </c>
       <c r="I11" t="n">
         <v>40744</v>
@@ -792,25 +792,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C12" t="n">
-        <v>16939.58112849111</v>
+        <v>16969.28617321799</v>
       </c>
       <c r="D12" t="n">
-        <v>12574.90819046136</v>
+        <v>12312.16610049215</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>6127</v>
+        <v>6532</v>
       </c>
       <c r="G12" t="n">
-        <v>13942</v>
+        <v>14595</v>
       </c>
       <c r="H12" t="n">
-        <v>27866</v>
+        <v>27149</v>
       </c>
       <c r="I12" t="n">
         <v>44461</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5574516957639453</v>
+        <v>0.5574502936142973</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5907856904234268</v>
+        <v>0.5908322098315822</v>
       </c>
       <c r="E13" t="n">
         <v>0.071936</v>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C14" t="n">
-        <v>23.89068987176934</v>
+        <v>23.88875381010272</v>
       </c>
       <c r="D14" t="n">
-        <v>13.41220079634299</v>
+        <v>13.41276591323907</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
@@ -885,13 +885,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6730256001715871</v>
+        <v>0.6732121148052223</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7486850399117433</v>
+        <v>0.7486168012273926</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C16" t="n">
-        <v>1.829825502121857</v>
+        <v>1.829788983444039</v>
       </c>
       <c r="D16" t="n">
-        <v>1.669206383178753</v>
+        <v>1.669302736950451</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -947,13 +947,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>326365</v>
+        <v>340542</v>
       </c>
       <c r="C17" t="n">
-        <v>93.70858701147495</v>
+        <v>93.73234079790458</v>
       </c>
       <c r="D17" t="n">
-        <v>23.56389603211523</v>
+        <v>23.56758322220557</v>
       </c>
       <c r="E17" t="n">
         <v>49.4</v>
@@ -978,22 +978,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>325815</v>
+        <v>339939</v>
       </c>
       <c r="C18" t="n">
-        <v>-85.49400906864766</v>
+        <v>-85.51379225515126</v>
       </c>
       <c r="D18" t="n">
-        <v>21.33243357679397</v>
+        <v>21.33041486398002</v>
       </c>
       <c r="E18" t="n">
         <v>-125.9574620641016</v>
       </c>
       <c r="F18" t="n">
-        <v>-102.3377954106368</v>
+        <v>-102.4139268515822</v>
       </c>
       <c r="G18" t="n">
-        <v>-85.14699179957641</v>
+        <v>-85.02214159641585</v>
       </c>
       <c r="H18" t="n">
         <v>-65.96183611348224</v>
@@ -1009,25 +1009,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>325815</v>
+        <v>339939</v>
       </c>
       <c r="C19" t="n">
-        <v>-77.7698309307473</v>
+        <v>-77.79296910746885</v>
       </c>
       <c r="D19" t="n">
-        <v>25.63065589012173</v>
+        <v>25.63942277324374</v>
       </c>
       <c r="E19" t="n">
         <v>-145.0217119216414</v>
       </c>
       <c r="F19" t="n">
-        <v>-92.61209675612977</v>
+        <v>-92.66683163887967</v>
       </c>
       <c r="G19" t="n">
-        <v>-74.3175485570292</v>
+        <v>-74.26572375596102</v>
       </c>
       <c r="H19" t="n">
-        <v>-55.25410721860875</v>
+        <v>-55.2778545523916</v>
       </c>
       <c r="I19" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Updates of IF NB
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C2" t="n">
-        <v>534.0941587234468</v>
+        <v>535.6390868169799</v>
       </c>
       <c r="D2" t="n">
-        <v>116.5276101818023</v>
+        <v>116.9466068346856</v>
       </c>
       <c r="E2" t="n">
         <v>390</v>
@@ -497,10 +497,10 @@
         <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="H2" t="n">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -513,25 +513,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C3" t="n">
-        <v>44.90025967428392</v>
+        <v>44.8323322096849</v>
       </c>
       <c r="D3" t="n">
-        <v>4.62925788268382</v>
+        <v>4.621473429827478</v>
       </c>
       <c r="E3" t="n">
         <v>30.48</v>
       </c>
       <c r="F3" t="n">
-        <v>41.45</v>
+        <v>41.4</v>
       </c>
       <c r="G3" t="n">
-        <v>44.84</v>
+        <v>44.73</v>
       </c>
       <c r="H3" t="n">
-        <v>48.12</v>
+        <v>48.06</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -544,25 +544,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C4" t="n">
-        <v>1.705674747901874</v>
+        <v>1.713164795681499</v>
       </c>
       <c r="D4" t="n">
-        <v>3.238081598277234</v>
+        <v>3.214947452006224</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="G4" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="H4" t="n">
-        <v>2.33</v>
+        <v>2.34</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -575,25 +575,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C5" t="n">
-        <v>322.5149398312103</v>
+        <v>322.7666752790618</v>
       </c>
       <c r="D5" t="n">
-        <v>9.867247193481946</v>
+        <v>9.953793745894442</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>318.08</v>
+        <v>318.25</v>
       </c>
       <c r="G5" t="n">
-        <v>324.39</v>
+        <v>324.55</v>
       </c>
       <c r="H5" t="n">
-        <v>329.84</v>
+        <v>330.13</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -606,25 +606,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C6" t="n">
-        <v>22.51477858825049</v>
+        <v>22.49146121394401</v>
       </c>
       <c r="D6" t="n">
-        <v>1.835523249557064</v>
+        <v>1.831778201666372</v>
       </c>
       <c r="E6" t="n">
         <v>15.83</v>
       </c>
       <c r="F6" t="n">
-        <v>21.52</v>
+        <v>21.5</v>
       </c>
       <c r="G6" t="n">
-        <v>22.19</v>
+        <v>22.18</v>
       </c>
       <c r="H6" t="n">
-        <v>23.13</v>
+        <v>23.09</v>
       </c>
       <c r="I6" t="n">
         <v>34.01</v>
@@ -637,13 +637,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C7" t="n">
-        <v>-76.33234079790452</v>
+        <v>-76.3445573219296</v>
       </c>
       <c r="D7" t="n">
-        <v>23.56758322221495</v>
+        <v>23.57114007655997</v>
       </c>
       <c r="E7" t="n">
         <v>-123</v>
@@ -668,13 +668,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>339939</v>
+        <v>346175</v>
       </c>
       <c r="C8" t="n">
-        <v>7.720823147682379</v>
+        <v>7.715290821116488</v>
       </c>
       <c r="D8" t="n">
-        <v>6.579145716284592</v>
+        <v>6.588808512354376</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C9" t="n">
-        <v>9.324559085222969</v>
+        <v>9.324986230741061</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688312520378005</v>
+        <v>1.68830073645217</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8304931550293</v>
+        <v>867.8305129661726</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4611783823689606</v>
+        <v>0.4611838944876139</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,25 +761,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>340530</v>
+        <v>346775</v>
       </c>
       <c r="C11" t="n">
-        <v>15176.54487416674</v>
+        <v>15218.6571927042</v>
       </c>
       <c r="D11" t="n">
-        <v>11053.5498440258</v>
+        <v>10958.08551391938</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>5787</v>
+        <v>5904.5</v>
       </c>
       <c r="G11" t="n">
-        <v>13032</v>
+        <v>13292</v>
       </c>
       <c r="H11" t="n">
-        <v>24291</v>
+        <v>24024</v>
       </c>
       <c r="I11" t="n">
         <v>40744</v>
@@ -792,25 +792,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C12" t="n">
-        <v>16969.28617321799</v>
+        <v>17015.43689353984</v>
       </c>
       <c r="D12" t="n">
-        <v>12312.16610049215</v>
+        <v>12205.64096082226</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>6532</v>
+        <v>6658</v>
       </c>
       <c r="G12" t="n">
-        <v>14595</v>
+        <v>14880</v>
       </c>
       <c r="H12" t="n">
-        <v>27149</v>
+        <v>26858</v>
       </c>
       <c r="I12" t="n">
         <v>44461</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5574502936142973</v>
+        <v>0.5575621475084129</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5908322098315822</v>
+        <v>0.5908465707913436</v>
       </c>
       <c r="E13" t="n">
         <v>0.071936</v>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C14" t="n">
-        <v>23.88875381010272</v>
+        <v>23.88641154368532</v>
       </c>
       <c r="D14" t="n">
-        <v>13.41276591323907</v>
+        <v>13.41248742079259</v>
       </c>
       <c r="E14" t="n">
         <v>8</v>
@@ -885,13 +885,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6732121148052223</v>
+        <v>0.6731826740910126</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7486168012273926</v>
+        <v>0.7485774219064837</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C16" t="n">
-        <v>1.829788983444039</v>
+        <v>1.829532248902064</v>
       </c>
       <c r="D16" t="n">
-        <v>1.669302736950451</v>
+        <v>1.66924279364245</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -947,13 +947,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>340542</v>
+        <v>346787</v>
       </c>
       <c r="C17" t="n">
-        <v>93.73234079790458</v>
+        <v>93.74455732192966</v>
       </c>
       <c r="D17" t="n">
-        <v>23.56758322220557</v>
+        <v>23.57114007656078</v>
       </c>
       <c r="E17" t="n">
         <v>49.4</v>
@@ -978,25 +978,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>339939</v>
+        <v>346175</v>
       </c>
       <c r="C18" t="n">
-        <v>-85.51379225515126</v>
+        <v>-85.52426874597096</v>
       </c>
       <c r="D18" t="n">
-        <v>21.33041486398002</v>
+        <v>21.33147651874848</v>
       </c>
       <c r="E18" t="n">
         <v>-125.9574620641016</v>
       </c>
       <c r="F18" t="n">
-        <v>-102.4139268515822</v>
+        <v>-102.4541072186088</v>
       </c>
       <c r="G18" t="n">
         <v>-85.02214159641585</v>
       </c>
       <c r="H18" t="n">
-        <v>-65.96183611348224</v>
+        <v>-66.07382219273629</v>
       </c>
       <c r="I18" t="n">
         <v>-33.14609373817283</v>
@@ -1009,25 +1009,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>339939</v>
+        <v>346175</v>
       </c>
       <c r="C19" t="n">
-        <v>-77.79296910746885</v>
+        <v>-77.80897792485445</v>
       </c>
       <c r="D19" t="n">
-        <v>25.63942277324374</v>
+        <v>25.65039259912822</v>
       </c>
       <c r="E19" t="n">
         <v>-145.0217119216414</v>
       </c>
       <c r="F19" t="n">
-        <v>-92.66683163887967</v>
+        <v>-92.71081852649533</v>
       </c>
       <c r="G19" t="n">
-        <v>-74.26572375596102</v>
+        <v>-74.25410721860875</v>
       </c>
       <c r="H19" t="n">
-        <v>-55.2778545523916</v>
+        <v>-55.29706163635328</v>
       </c>
       <c r="I19" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Updates EDA and STATS NB.
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,55 +434,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Field</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>Unit</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>mean</t>
+          <t>Mean</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>std</t>
+          <t>STD (σ)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>min</t>
+          <t>Min</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>1ˢᵗ Quartile (25%)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>Median</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>3ʳᵈ Quartile (75%)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>max</t>
+          <t>Max</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>co2</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>346787</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ppm</t>
+        </is>
       </c>
       <c r="C2" t="n">
         <v>535.6390868169799</v>
@@ -507,13 +514,15 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>humidity</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>346787</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
       </c>
       <c r="C3" t="n">
         <v>44.8323322096849</v>
@@ -538,13 +547,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>pm25</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>346787</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>µg/m³</t>
+        </is>
       </c>
       <c r="C4" t="n">
         <v>1.713164795681499</v>
@@ -569,13 +580,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>pressure</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>346787</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>hPa</t>
+        </is>
       </c>
       <c r="C5" t="n">
         <v>322.7666752790618</v>
@@ -600,13 +613,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>temperature</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>346787</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
       </c>
       <c r="C6" t="n">
         <v>22.49146121394401</v>
@@ -631,13 +646,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>rssi</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>346787</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dBm</t>
+        </is>
       </c>
       <c r="C7" t="n">
         <v>-76.3445573219296</v>
@@ -662,13 +679,15 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>snr</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>346175</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dB</t>
+        </is>
       </c>
       <c r="C8" t="n">
         <v>7.715290821116488</v>
@@ -693,13 +712,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>346787</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>bit/sym</t>
+        </is>
       </c>
       <c r="C9" t="n">
         <v>9.324986230741061</v>
@@ -724,13 +745,15 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>frequency</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>346787</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MHz</t>
+        </is>
       </c>
       <c r="C10" t="n">
         <v>867.8305129661726</v>
@@ -755,281 +778,225 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>f_count</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>346775</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>toa</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>15218.6571927042</v>
+        <v>0.5575621475084129</v>
       </c>
       <c r="D11" t="n">
-        <v>10958.08551391938</v>
+        <v>0.5908465707913436</v>
       </c>
       <c r="E11" t="n">
+        <v>0.071936</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.133632</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.246784</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.987136</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.974272</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>distance</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>23.88641154368532</v>
+      </c>
+      <c r="D12" t="n">
+        <v>13.41248742079259</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>25</v>
+      </c>
+      <c r="H12" t="n">
+        <v>39</v>
+      </c>
+      <c r="I12" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>c_walls</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0.6731826740910126</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.7485774219064837</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
         <v>1</v>
       </c>
-      <c r="F11" t="n">
-        <v>5904.5</v>
-      </c>
-      <c r="G11" t="n">
-        <v>13292</v>
-      </c>
-      <c r="H11" t="n">
-        <v>24024</v>
-      </c>
-      <c r="I11" t="n">
-        <v>40744</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>p_count</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>346787</v>
-      </c>
-      <c r="C12" t="n">
-        <v>17015.43689353984</v>
-      </c>
-      <c r="D12" t="n">
-        <v>12205.64096082226</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>w_walls</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>1.829532248902064</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.66924279364245</v>
+      </c>
+      <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="n">
-        <v>6658</v>
-      </c>
-      <c r="G12" t="n">
-        <v>14880</v>
-      </c>
-      <c r="H12" t="n">
-        <v>26858</v>
-      </c>
-      <c r="I12" t="n">
-        <v>44461</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>toa</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>346787</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.5575621475084129</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.5908465707913436</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.071936</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.133632</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.246784</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.987136</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1.974272</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>distance</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>346787</v>
-      </c>
-      <c r="C14" t="n">
-        <v>23.88641154368532</v>
-      </c>
-      <c r="D14" t="n">
-        <v>13.41248742079259</v>
-      </c>
-      <c r="E14" t="n">
-        <v>8</v>
-      </c>
       <c r="F14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="H14" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>c_walls</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>346787</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>exp_pl</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>dB</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6731826740910126</v>
+        <v>93.74455732192966</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7485774219064837</v>
+        <v>23.57114007656078</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>49.4</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>109.4</v>
       </c>
       <c r="I15" t="n">
-        <v>2</v>
+        <v>140.4</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>w_walls</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>346787</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>n_power</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>dB</t>
+        </is>
       </c>
       <c r="C16" t="n">
-        <v>1.829532248902064</v>
+        <v>-85.52426874597096</v>
       </c>
       <c r="D16" t="n">
-        <v>1.66924279364245</v>
+        <v>21.33147651874848</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>-125.9574620641016</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>-102.4541072186088</v>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>-85.02214159641585</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>-66.07382219273629</v>
       </c>
       <c r="I16" t="n">
-        <v>5</v>
+        <v>-33.14609373817283</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>exp_pl</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>346787</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>esp</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>dBm</t>
+        </is>
       </c>
       <c r="C17" t="n">
-        <v>93.74455732192966</v>
+        <v>-77.80897792485445</v>
       </c>
       <c r="D17" t="n">
-        <v>23.57114007656078</v>
+        <v>25.65039259912822</v>
       </c>
       <c r="E17" t="n">
-        <v>49.4</v>
+        <v>-145.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>72.40000000000001</v>
+        <v>-92.71081852649533</v>
       </c>
       <c r="G17" t="n">
-        <v>91.40000000000001</v>
+        <v>-74.25410721860875</v>
       </c>
       <c r="H17" t="n">
-        <v>109.4</v>
+        <v>-55.29706163635328</v>
       </c>
       <c r="I17" t="n">
-        <v>140.4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>n_power</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>346175</v>
-      </c>
-      <c r="C18" t="n">
-        <v>-85.52426874597096</v>
-      </c>
-      <c r="D18" t="n">
-        <v>21.33147651874848</v>
-      </c>
-      <c r="E18" t="n">
-        <v>-125.9574620641016</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-102.4541072186088</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-85.02214159641585</v>
-      </c>
-      <c r="H18" t="n">
-        <v>-66.07382219273629</v>
-      </c>
-      <c r="I18" t="n">
-        <v>-33.14609373817283</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>esp</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>346175</v>
-      </c>
-      <c r="C19" t="n">
-        <v>-77.80897792485445</v>
-      </c>
-      <c r="D19" t="n">
-        <v>25.65039259912822</v>
-      </c>
-      <c r="E19" t="n">
-        <v>-145.0217119216414</v>
-      </c>
-      <c r="F19" t="n">
-        <v>-92.71081852649533</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-74.25410721860875</v>
-      </c>
-      <c r="H19" t="n">
-        <v>-55.29706163635328</v>
-      </c>
-      <c r="I19" t="n">
         <v>-33.49305820175223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More Data, Path Loss Simulation NB and General Updates
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>535.6390868169799</v>
+        <v>539.7372594187245</v>
       </c>
       <c r="D2" t="n">
-        <v>116.9466068346856</v>
+        <v>120.6474353692902</v>
       </c>
       <c r="E2" t="n">
         <v>390</v>
@@ -504,10 +504,10 @@
         <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="H2" t="n">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>44.8323322096849</v>
+        <v>44.17396072102088</v>
       </c>
       <c r="D3" t="n">
-        <v>4.621473429827478</v>
+        <v>4.758166755696192</v>
       </c>
       <c r="E3" t="n">
         <v>30.48</v>
       </c>
       <c r="F3" t="n">
-        <v>41.4</v>
+        <v>40.77</v>
       </c>
       <c r="G3" t="n">
-        <v>44.73</v>
+        <v>44.18</v>
       </c>
       <c r="H3" t="n">
-        <v>48.06</v>
+        <v>47.46</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.713164795681499</v>
+        <v>1.719347887877447</v>
       </c>
       <c r="D4" t="n">
-        <v>3.214947452006224</v>
+        <v>3.034312183912127</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="G4" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="H4" t="n">
-        <v>2.34</v>
+        <v>2.32</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.7666752790618</v>
+        <v>324.1342573648086</v>
       </c>
       <c r="D5" t="n">
-        <v>9.953793745894442</v>
+        <v>9.839614067400744</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>318.25</v>
+        <v>319.48</v>
       </c>
       <c r="G5" t="n">
-        <v>324.55</v>
+        <v>325.9</v>
       </c>
       <c r="H5" t="n">
-        <v>330.13</v>
+        <v>331.43</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22.49146121394401</v>
+        <v>22.32895665520659</v>
       </c>
       <c r="D6" t="n">
-        <v>1.831778201666372</v>
+        <v>1.905973564937634</v>
       </c>
       <c r="E6" t="n">
         <v>15.83</v>
       </c>
       <c r="F6" t="n">
-        <v>21.5</v>
+        <v>21.26</v>
       </c>
       <c r="G6" t="n">
-        <v>22.18</v>
+        <v>22.1</v>
       </c>
       <c r="H6" t="n">
-        <v>23.09</v>
+        <v>23</v>
       </c>
       <c r="I6" t="n">
         <v>34.01</v>
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.3445573219296</v>
+        <v>-76.54445825805192</v>
       </c>
       <c r="D7" t="n">
-        <v>23.57114007655997</v>
+        <v>23.67145994587697</v>
       </c>
       <c r="E7" t="n">
-        <v>-123</v>
+        <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-92</v>
+        <v>-93</v>
       </c>
       <c r="G7" t="n">
         <v>-74</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.715290821116488</v>
+        <v>7.603666585792167</v>
       </c>
       <c r="D8" t="n">
-        <v>6.588808512354376</v>
+        <v>6.778738504416467</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.324986230741061</v>
+        <v>9.323404013415951</v>
       </c>
       <c r="D9" t="n">
-        <v>1.68830073645217</v>
+        <v>1.688146978757465</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8305129661726</v>
+        <v>867.8305786308711</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4611838944876139</v>
+        <v>0.4612136517686191</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5575621475084129</v>
+        <v>0.5570904454402326</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5908465707913436</v>
+        <v>0.590697459462397</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>23.88641154368532</v>
+        <v>23.89064813281495</v>
       </c>
       <c r="D12" t="n">
-        <v>13.41248742079259</v>
+        <v>13.40902774681995</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6731826740910126</v>
+        <v>0.6728366531304298</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7485774219064837</v>
+        <v>0.7487252749585708</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.829532248902064</v>
+        <v>1.82979191434355</v>
       </c>
       <c r="D14" t="n">
-        <v>1.66924279364245</v>
+        <v>1.668613383530017</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.74455732192966</v>
+        <v>93.94445825805194</v>
       </c>
       <c r="D15" t="n">
-        <v>23.57114007656078</v>
+        <v>23.67145994588451</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -928,10 +928,10 @@
         <v>91.40000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>109.4</v>
+        <v>110.4</v>
       </c>
       <c r="I15" t="n">
-        <v>140.4</v>
+        <v>145.4</v>
       </c>
     </row>
     <row r="16">
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.52426874597096</v>
+        <v>-85.68788297974999</v>
       </c>
       <c r="D16" t="n">
-        <v>21.33147651874848</v>
+        <v>21.36988236077568</v>
       </c>
       <c r="E16" t="n">
-        <v>-125.9574620641016</v>
+        <v>-136.4668316388797</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.4541072186088</v>
+        <v>-102.7643486243649</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.02214159641585</v>
+        <v>-84.59612087980607</v>
       </c>
       <c r="H16" t="n">
-        <v>-66.07382219273629</v>
+        <v>-66.0778545523916</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.80897792485445</v>
+        <v>-78.08421639395782</v>
       </c>
       <c r="D17" t="n">
-        <v>25.65039259912822</v>
+        <v>25.88602677945289</v>
       </c>
       <c r="E17" t="n">
-        <v>-145.0217119216414</v>
+        <v>-145.8227324995171</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.71081852649533</v>
+        <v>-93.3707776445072</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.25410721860875</v>
+        <v>-74.1773721860196</v>
       </c>
       <c r="H17" t="n">
-        <v>-55.29706163635328</v>
+        <v>-55.26572375596102</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
MORE DATA AND NEW MODEL EQUATIONS/PARAMETERS
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>539.7372594187245</v>
+        <v>539.8645649892381</v>
       </c>
       <c r="D2" t="n">
-        <v>120.6474353692902</v>
+        <v>121.3843902993817</v>
       </c>
       <c r="E2" t="n">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G2" t="n">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="H2" t="n">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>44.17396072102088</v>
+        <v>43.71295319921021</v>
       </c>
       <c r="D3" t="n">
-        <v>4.758166755696192</v>
+        <v>4.81069944699828</v>
       </c>
       <c r="E3" t="n">
         <v>30.48</v>
       </c>
       <c r="F3" t="n">
-        <v>40.77</v>
+        <v>40.42</v>
       </c>
       <c r="G3" t="n">
-        <v>44.18</v>
+        <v>43.65</v>
       </c>
       <c r="H3" t="n">
-        <v>47.46</v>
+        <v>46.93</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.719347887877447</v>
+        <v>1.634615819058292</v>
       </c>
       <c r="D4" t="n">
-        <v>3.034312183912127</v>
+        <v>2.899470628101848</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.65</v>
+        <v>0.59</v>
       </c>
       <c r="G4" t="n">
-        <v>1.33</v>
+        <v>1.24</v>
       </c>
       <c r="H4" t="n">
-        <v>2.32</v>
+        <v>2.22</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>324.1342573648086</v>
+        <v>323.2238041873454</v>
       </c>
       <c r="D5" t="n">
-        <v>9.839614067400744</v>
+        <v>10.29980121078036</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>319.48</v>
+        <v>317.83</v>
       </c>
       <c r="G5" t="n">
-        <v>325.9</v>
+        <v>325.28</v>
       </c>
       <c r="H5" t="n">
-        <v>331.43</v>
+        <v>331.07</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22.32895665520659</v>
+        <v>22.25705242631233</v>
       </c>
       <c r="D6" t="n">
-        <v>1.905973564937634</v>
+        <v>1.91375967437697</v>
       </c>
       <c r="E6" t="n">
         <v>15.83</v>
       </c>
       <c r="F6" t="n">
-        <v>21.26</v>
+        <v>21.12</v>
       </c>
       <c r="G6" t="n">
-        <v>22.1</v>
+        <v>22.05</v>
       </c>
       <c r="H6" t="n">
-        <v>23</v>
+        <v>22.95</v>
       </c>
       <c r="I6" t="n">
         <v>34.01</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.54445825805192</v>
+        <v>-76.67362852873686</v>
       </c>
       <c r="D7" t="n">
-        <v>23.67145994587697</v>
+        <v>23.63823620582192</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.603666585792167</v>
+        <v>7.572089589466981</v>
       </c>
       <c r="D8" t="n">
-        <v>6.778738504416467</v>
+        <v>6.818340091312328</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="G8" t="n">
         <v>9.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.323404013415951</v>
+        <v>9.323242969208602</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688146978757465</v>
+        <v>1.688459102614802</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8305786308711</v>
+        <v>867.8304938897485</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4612136517686191</v>
+        <v>0.4612111841487337</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5570904454402326</v>
+        <v>0.5571688973797961</v>
       </c>
       <c r="D11" t="n">
-        <v>0.590697459462397</v>
+        <v>0.5908796707351528</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>23.89064813281495</v>
+        <v>22.71885506163616</v>
       </c>
       <c r="D12" t="n">
-        <v>13.40902774681995</v>
+        <v>12.2909692008134</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -834,13 +834,13 @@
         <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H12" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I12" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6728366531304298</v>
+        <v>0.6726990945799314</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7487252749585708</v>
+        <v>0.7488468742878095</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.82979191434355</v>
+        <v>1.829617820232314</v>
       </c>
       <c r="D14" t="n">
-        <v>1.668613383530017</v>
+        <v>1.668499562659637</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.94445825805194</v>
+        <v>94.07362852873686</v>
       </c>
       <c r="D15" t="n">
-        <v>23.67145994588451</v>
+        <v>23.63823620581789</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.68788297974999</v>
+        <v>-85.80559799117486</v>
       </c>
       <c r="D16" t="n">
-        <v>21.36988236077568</v>
+        <v>21.31908538193078</v>
       </c>
       <c r="E16" t="n">
         <v>-136.4668316388797</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.7643486243649</v>
+        <v>-102.9618361134822</v>
       </c>
       <c r="G16" t="n">
         <v>-84.59612087980607</v>
       </c>
       <c r="H16" t="n">
-        <v>-66.0778545523916</v>
+        <v>-66.14699179957641</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.08421639395782</v>
+        <v>-78.23350840170788</v>
       </c>
       <c r="D17" t="n">
-        <v>25.88602677945289</v>
+        <v>25.88644199732135</v>
       </c>
       <c r="E17" t="n">
         <v>-145.8227324995171</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.3707776445072</v>
+        <v>-93.49305820175223</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.1773721860196</v>
+        <v>-74.18978441047734</v>
       </c>
       <c r="H17" t="n">
         <v>-55.26572375596102</v>

</xml_diff>

<commit_message>
Update on MODELING COMMON TEST SPLIT
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>539.8645649892381</v>
+        <v>538.1254780066262</v>
       </c>
       <c r="D2" t="n">
-        <v>121.3843902993817</v>
+        <v>120.1197662093448</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G2" t="n">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H2" t="n">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>43.71295319921021</v>
+        <v>43.19081207395062</v>
       </c>
       <c r="D3" t="n">
-        <v>4.81069944699828</v>
+        <v>5.001223665698476</v>
       </c>
       <c r="E3" t="n">
-        <v>30.48</v>
+        <v>28.54</v>
       </c>
       <c r="F3" t="n">
-        <v>40.42</v>
+        <v>39.77</v>
       </c>
       <c r="G3" t="n">
-        <v>43.65</v>
+        <v>43.1</v>
       </c>
       <c r="H3" t="n">
-        <v>46.93</v>
+        <v>46.59</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.634615819058292</v>
+        <v>1.564071704035329</v>
       </c>
       <c r="D4" t="n">
-        <v>2.899470628101848</v>
+        <v>2.784652578677638</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.59</v>
+        <v>0.57</v>
       </c>
       <c r="G4" t="n">
-        <v>1.24</v>
+        <v>1.16</v>
       </c>
       <c r="H4" t="n">
-        <v>2.22</v>
+        <v>2.1</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.2238041873454</v>
+        <v>322.3611026898137</v>
       </c>
       <c r="D5" t="n">
-        <v>10.29980121078036</v>
+        <v>10.44548591421454</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.83</v>
+        <v>315.98</v>
       </c>
       <c r="G5" t="n">
-        <v>325.28</v>
+        <v>324.38</v>
       </c>
       <c r="H5" t="n">
-        <v>331.07</v>
+        <v>330.69</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22.25705242631233</v>
+        <v>22.11743291686436</v>
       </c>
       <c r="D6" t="n">
-        <v>1.91375967437697</v>
+        <v>1.942015821583213</v>
       </c>
       <c r="E6" t="n">
         <v>15.83</v>
       </c>
       <c r="F6" t="n">
-        <v>21.12</v>
+        <v>20.91</v>
       </c>
       <c r="G6" t="n">
-        <v>22.05</v>
+        <v>21.96</v>
       </c>
       <c r="H6" t="n">
-        <v>22.95</v>
+        <v>22.87</v>
       </c>
       <c r="I6" t="n">
         <v>34.01</v>
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.67362852873686</v>
+        <v>-76.83377129486571</v>
       </c>
       <c r="D7" t="n">
-        <v>23.63823620582192</v>
+        <v>23.67980839532934</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-93</v>
+        <v>-94</v>
       </c>
       <c r="G7" t="n">
         <v>-74</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.572089589466981</v>
+        <v>7.519434189096432</v>
       </c>
       <c r="D8" t="n">
-        <v>6.818340091312328</v>
+        <v>6.887967962223891</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.323242969208602</v>
+        <v>9.32322169369457</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688459102614802</v>
+        <v>1.688405586861373</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8304938897485</v>
+        <v>867.8304302161014</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4612111841487337</v>
+        <v>0.4613076307960154</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5571688973797961</v>
+        <v>0.5571491068585587</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5908796707351528</v>
+        <v>0.5908570403400689</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.71885506163616</v>
+        <v>22.71709509848052</v>
       </c>
       <c r="D12" t="n">
-        <v>12.2909692008134</v>
+        <v>12.2911372628886</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6726990945799314</v>
+        <v>0.6725933405515883</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7488468742878095</v>
+        <v>0.7488690246624591</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.829617820232314</v>
+        <v>1.829280161559143</v>
       </c>
       <c r="D14" t="n">
-        <v>1.668499562659637</v>
+        <v>1.66849122640517</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>94.07362852873686</v>
+        <v>94.23377129486568</v>
       </c>
       <c r="D15" t="n">
-        <v>23.63823620581789</v>
+        <v>23.67980839532417</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -928,7 +928,7 @@
         <v>91.40000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>110.4</v>
+        <v>111.4</v>
       </c>
       <c r="I15" t="n">
         <v>145.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.80559799117486</v>
+        <v>-85.94257698204969</v>
       </c>
       <c r="D16" t="n">
-        <v>21.31908538193078</v>
+        <v>21.33025101082983</v>
       </c>
       <c r="E16" t="n">
-        <v>-136.4668316388797</v>
+        <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.9618361134822</v>
+        <v>-103.3377954106368</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.59612087980607</v>
+        <v>-84.69305820175224</v>
       </c>
       <c r="H16" t="n">
-        <v>-66.14699179957641</v>
+        <v>-66.33195619988427</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.23350840170788</v>
+        <v>-78.42314279295324</v>
       </c>
       <c r="D17" t="n">
-        <v>25.88644199732135</v>
+        <v>25.97442681196299</v>
       </c>
       <c r="E17" t="n">
         <v>-145.8227324995171</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.49305820175223</v>
+        <v>-93.93380807687734</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.18978441047734</v>
+        <v>-74.21238401914255</v>
       </c>
       <c r="H17" t="n">
-        <v>-55.26572375596102</v>
+        <v>-55.43249407632486</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
General but minor updates on warnings such of legend locs
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>542.3780982010798</v>
+        <v>552.5041813615475</v>
       </c>
       <c r="D2" t="n">
-        <v>126.7359587154584</v>
+        <v>133.2343220950599</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G2" t="n">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="H2" t="n">
-        <v>605</v>
+        <v>619</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>42.00618521082122</v>
+        <v>41.64199416212463</v>
       </c>
       <c r="D3" t="n">
-        <v>4.816168163467332</v>
+        <v>4.854508218915211</v>
       </c>
       <c r="E3" t="n">
         <v>24.86</v>
       </c>
       <c r="F3" t="n">
-        <v>38.69</v>
+        <v>38.55</v>
       </c>
       <c r="G3" t="n">
-        <v>41.01</v>
+        <v>40.66</v>
       </c>
       <c r="H3" t="n">
-        <v>45.07</v>
+        <v>44.65</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.384315616142923</v>
+        <v>1.350393341883082</v>
       </c>
       <c r="D4" t="n">
-        <v>2.426046859031906</v>
+        <v>2.332899451123587</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="G4" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="H4" t="n">
-        <v>1.8</v>
+        <v>1.73</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>321.1805827073421</v>
+        <v>321.9401196296889</v>
       </c>
       <c r="D5" t="n">
-        <v>10.38059120860663</v>
+        <v>10.27790085095419</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>314.39</v>
+        <v>315.36</v>
       </c>
       <c r="G5" t="n">
-        <v>322.68</v>
+        <v>323.87</v>
       </c>
       <c r="H5" t="n">
-        <v>329.87</v>
+        <v>330.37</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.61027099651</v>
+        <v>21.52157452976382</v>
       </c>
       <c r="D6" t="n">
-        <v>2.002040969143651</v>
+        <v>2.003594379020124</v>
       </c>
       <c r="E6" t="n">
         <v>15.53</v>
       </c>
       <c r="F6" t="n">
-        <v>20.17</v>
+        <v>20.05</v>
       </c>
       <c r="G6" t="n">
-        <v>21.49</v>
+        <v>21.36</v>
       </c>
       <c r="H6" t="n">
-        <v>22.52</v>
+        <v>22.47</v>
       </c>
       <c r="I6" t="n">
         <v>34.09</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.28743378822432</v>
+        <v>-76.19348081650101</v>
       </c>
       <c r="D7" t="n">
-        <v>23.25291741098411</v>
+        <v>23.09578817080914</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.639440573316056</v>
+        <v>7.686607516620905</v>
       </c>
       <c r="D8" t="n">
-        <v>6.941520729957332</v>
+        <v>6.89608249706923</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322805994943497</v>
+        <v>9.322246713690285</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688824873582543</v>
+        <v>1.688607784523832</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8302499836064</v>
+        <v>867.8303182109649</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461282302846211</v>
+        <v>0.4611200429001951</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.557202721430393</v>
+        <v>0.5569688428342418</v>
       </c>
       <c r="D11" t="n">
-        <v>0.590999346108273</v>
+        <v>0.5908372583519632</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.71094871365183</v>
+        <v>22.70849898471732</v>
       </c>
       <c r="D12" t="n">
-        <v>12.28784793601912</v>
+        <v>12.28637657221718</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.672597978855948</v>
+        <v>0.6722988137223469</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7489712039830542</v>
+        <v>0.7488477031850275</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.82761987336884</v>
+        <v>1.827625040076948</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666981376133356</v>
+        <v>1.667054721662187</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.6874337882242</v>
+        <v>93.59348081650087</v>
       </c>
       <c r="D15" t="n">
-        <v>23.25291741100779</v>
+        <v>23.09578817080798</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,19 +946,19 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.52166488516276</v>
+        <v>-85.45703572767513</v>
       </c>
       <c r="D16" t="n">
-        <v>20.98380121403654</v>
+        <v>20.85876560659655</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.2324940763249</v>
+        <v>-101.8707776445072</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.7376019773414</v>
+        <v>-85.0778545523916</v>
       </c>
       <c r="H16" t="n">
         <v>-66.0778545523916</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.88222431184668</v>
+        <v>-77.77042821105421</v>
       </c>
       <c r="D17" t="n">
-        <v>25.63455628089887</v>
+        <v>25.46089467460196</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.79009749652566</v>
+        <v>-92.53779541063678</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.2778545523916</v>
+        <v>-74.46183611348224</v>
       </c>
       <c r="H17" t="n">
-        <v>-55.25410721860875</v>
+        <v>-54.79009749652566</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
on ANOMALIES and Modeling too.
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>552.5041813615475</v>
+        <v>561.6908063895213</v>
       </c>
       <c r="D2" t="n">
-        <v>133.2343220950599</v>
+        <v>133.3636251146518</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="G2" t="n">
-        <v>517</v>
+        <v>532</v>
       </c>
       <c r="H2" t="n">
-        <v>619</v>
+        <v>635</v>
       </c>
       <c r="I2" t="n">
         <v>1593</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41.64199416212463</v>
+        <v>41.00357317009417</v>
       </c>
       <c r="D3" t="n">
-        <v>4.854508218915211</v>
+        <v>5.038087600419884</v>
       </c>
       <c r="E3" t="n">
         <v>24.86</v>
       </c>
       <c r="F3" t="n">
-        <v>38.55</v>
+        <v>38.05</v>
       </c>
       <c r="G3" t="n">
-        <v>40.66</v>
+        <v>40.14</v>
       </c>
       <c r="H3" t="n">
-        <v>44.65</v>
+        <v>44.18</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.350393341883082</v>
+        <v>1.418916017527934</v>
       </c>
       <c r="D4" t="n">
-        <v>2.332899451123587</v>
+        <v>2.246730416347243</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
       <c r="G4" t="n">
-        <v>0.98</v>
+        <v>1.06</v>
       </c>
       <c r="H4" t="n">
-        <v>1.73</v>
+        <v>1.87</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>321.9401196296889</v>
+        <v>323.0147241417824</v>
       </c>
       <c r="D5" t="n">
-        <v>10.27790085095419</v>
+        <v>10.23774700587594</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>315.36</v>
+        <v>316.93</v>
       </c>
       <c r="G5" t="n">
-        <v>323.87</v>
+        <v>324.96</v>
       </c>
       <c r="H5" t="n">
-        <v>330.37</v>
+        <v>331.39</v>
       </c>
       <c r="I5" t="n">
         <v>342</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.52157452976382</v>
+        <v>21.38153595175066</v>
       </c>
       <c r="D6" t="n">
-        <v>2.003594379020124</v>
+        <v>2.018052522979711</v>
       </c>
       <c r="E6" t="n">
         <v>15.53</v>
       </c>
       <c r="F6" t="n">
-        <v>20.05</v>
+        <v>19.78</v>
       </c>
       <c r="G6" t="n">
-        <v>21.36</v>
+        <v>21.15</v>
       </c>
       <c r="H6" t="n">
-        <v>22.47</v>
+        <v>22.38</v>
       </c>
       <c r="I6" t="n">
         <v>34.09</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.19348081650101</v>
+        <v>-76.36750440812331</v>
       </c>
       <c r="D7" t="n">
-        <v>23.09578817080914</v>
+        <v>22.84409436797995</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,10 +669,10 @@
         <v>-92</v>
       </c>
       <c r="G7" t="n">
-        <v>-74</v>
+        <v>-75</v>
       </c>
       <c r="H7" t="n">
-        <v>-55</v>
+        <v>-56</v>
       </c>
       <c r="I7" t="n">
         <v>-32</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.686607516620905</v>
+        <v>7.705910763377934</v>
       </c>
       <c r="D8" t="n">
-        <v>6.89608249706923</v>
+        <v>6.887995004726862</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322246713690285</v>
+        <v>9.321625468734405</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688607784523832</v>
+        <v>1.689066655511287</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8303182109649</v>
+        <v>867.8305051638014</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4611200429001951</v>
+        <v>0.4610278333245824</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569688428342418</v>
+        <v>0.5569541734257892</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5908372583519632</v>
+        <v>0.5909813791365603</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.70849898471732</v>
+        <v>22.70173996112297</v>
       </c>
       <c r="D12" t="n">
-        <v>12.28637657221718</v>
+        <v>12.28042894373855</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6722988137223469</v>
+        <v>0.6727105086807948</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7488477031850275</v>
+        <v>0.748781494070802</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.827625040076948</v>
+        <v>1.826308060093058</v>
       </c>
       <c r="D14" t="n">
-        <v>1.667054721662187</v>
+        <v>1.665016986672359</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,19 +913,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.59348081650087</v>
+        <v>93.76750440812313</v>
       </c>
       <c r="D15" t="n">
-        <v>23.09578817080798</v>
+        <v>22.84409436798105</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
       </c>
       <c r="F15" t="n">
-        <v>72.40000000000001</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>91.40000000000001</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>109.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.45703572767513</v>
+        <v>-85.64339072166538</v>
       </c>
       <c r="D16" t="n">
-        <v>20.85876560659655</v>
+        <v>20.62162584814459</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.8707776445072</v>
+        <v>-101.6389203414338</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.0778545523916</v>
+        <v>-85.79706163635328</v>
       </c>
       <c r="H16" t="n">
-        <v>-66.0778545523916</v>
+        <v>-66.7376019773414</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.77042821105421</v>
+        <v>-77.93747995828738</v>
       </c>
       <c r="D17" t="n">
-        <v>25.46089467460196</v>
+        <v>25.21584035225402</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.53779541063678</v>
+        <v>-92.46183611348224</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.46183611348224</v>
+        <v>-75.41392685158225</v>
       </c>
       <c r="H17" t="n">
-        <v>-54.79009749652566</v>
+        <v>-56.2376019773414</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
General Updates: Notebook Cleaning, Taking care of warnings etc.
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,25 +492,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>561.6908063895213</v>
+        <v>555.9727745343941</v>
       </c>
       <c r="D2" t="n">
-        <v>133.3636251146518</v>
+        <v>136.4468106118986</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G2" t="n">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="H2" t="n">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="I2" t="n">
-        <v>1593</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="3">
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41.00357317009417</v>
+        <v>40.66421552496731</v>
       </c>
       <c r="D3" t="n">
-        <v>5.038087600419884</v>
+        <v>4.785040199674193</v>
       </c>
       <c r="E3" t="n">
         <v>24.86</v>
       </c>
       <c r="F3" t="n">
-        <v>38.05</v>
+        <v>37.69</v>
       </c>
       <c r="G3" t="n">
-        <v>40.14</v>
+        <v>39.94</v>
       </c>
       <c r="H3" t="n">
-        <v>44.18</v>
+        <v>43.35</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.418916017527934</v>
+        <v>1.386957574319462</v>
       </c>
       <c r="D4" t="n">
-        <v>2.246730416347243</v>
+        <v>2.251972007438511</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
       <c r="G4" t="n">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
       <c r="H4" t="n">
-        <v>1.87</v>
+        <v>1.79</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,25 +591,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.0147241417824</v>
+        <v>323.8454538002499</v>
       </c>
       <c r="D5" t="n">
-        <v>10.23774700587594</v>
+        <v>10.23904542492872</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.93</v>
+        <v>317.99</v>
       </c>
       <c r="G5" t="n">
-        <v>324.96</v>
+        <v>325.67</v>
       </c>
       <c r="H5" t="n">
-        <v>331.39</v>
+        <v>332.25</v>
       </c>
       <c r="I5" t="n">
-        <v>342</v>
+        <v>342.81</v>
       </c>
     </row>
     <row r="6">
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.38153595175066</v>
+        <v>21.03396809739433</v>
       </c>
       <c r="D6" t="n">
-        <v>2.018052522979711</v>
+        <v>2.100131944092435</v>
       </c>
       <c r="E6" t="n">
-        <v>15.53</v>
+        <v>15.22</v>
       </c>
       <c r="F6" t="n">
-        <v>19.78</v>
+        <v>19.48</v>
       </c>
       <c r="G6" t="n">
-        <v>21.15</v>
+        <v>20.66</v>
       </c>
       <c r="H6" t="n">
-        <v>22.38</v>
+        <v>22.2</v>
       </c>
       <c r="I6" t="n">
         <v>34.09</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.36750440812331</v>
+        <v>-76.31486173511111</v>
       </c>
       <c r="D7" t="n">
-        <v>22.84409436797995</v>
+        <v>22.43087720017906</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.705910763377934</v>
+        <v>7.772729262699947</v>
       </c>
       <c r="D8" t="n">
-        <v>6.887995004726862</v>
+        <v>6.826958247165576</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.321625468734405</v>
+        <v>9.322383399976859</v>
       </c>
       <c r="D9" t="n">
-        <v>1.689066655511287</v>
+        <v>1.688459844100303</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8305051638014</v>
+        <v>867.8303429706599</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4610278333245824</v>
+        <v>0.4610121929352152</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569541734257892</v>
+        <v>0.5569302727017788</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5909813791365603</v>
+        <v>0.5906666965420388</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.70173996112297</v>
+        <v>22.69027919682621</v>
       </c>
       <c r="D12" t="n">
-        <v>12.28042894373855</v>
+        <v>12.27804715606286</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6727105086807948</v>
+        <v>0.6716804562221651</v>
       </c>
       <c r="D13" t="n">
-        <v>0.748781494070802</v>
+        <v>0.7483016417848986</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826308060093058</v>
+        <v>1.826072163270429</v>
       </c>
       <c r="D14" t="n">
-        <v>1.665016986672359</v>
+        <v>1.665922424560786</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.76750440812313</v>
+        <v>93.71486173511092</v>
       </c>
       <c r="D15" t="n">
-        <v>22.84409436798105</v>
+        <v>22.43087720014354</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.64339072166538</v>
+        <v>-85.63531770634948</v>
       </c>
       <c r="D16" t="n">
-        <v>20.62162584814459</v>
+        <v>20.23553674694372</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.6389203414338</v>
+        <v>-101.0778545523916</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.79706163635328</v>
+        <v>-85.69305820175224</v>
       </c>
       <c r="H16" t="n">
-        <v>-66.7376019773414</v>
+        <v>-67.59612087980607</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.93747995828738</v>
+        <v>-77.86258844364953</v>
       </c>
       <c r="D17" t="n">
-        <v>25.21584035225402</v>
+        <v>24.79941101361801</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.46183611348224</v>
+        <v>-92.22214159641585</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.41392685158225</v>
+        <v>-75.43249407632486</v>
       </c>
       <c r="H17" t="n">
-        <v>-56.2376019773414</v>
+        <v>-56.66683163887967</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
General Updates with more data used
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>555.9727745343941</v>
+        <v>555.3976844498427</v>
       </c>
       <c r="D2" t="n">
-        <v>136.4468106118986</v>
+        <v>136.1086402776294</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
@@ -504,10 +504,10 @@
         <v>452</v>
       </c>
       <c r="G2" t="n">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H2" t="n">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.66421552496731</v>
+        <v>40.65229553045877</v>
       </c>
       <c r="D3" t="n">
-        <v>4.785040199674193</v>
+        <v>4.778124445764926</v>
       </c>
       <c r="E3" t="n">
         <v>24.86</v>
       </c>
       <c r="F3" t="n">
-        <v>37.69</v>
+        <v>37.68</v>
       </c>
       <c r="G3" t="n">
         <v>39.94</v>
       </c>
       <c r="H3" t="n">
-        <v>43.35</v>
+        <v>43.32</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.386957574319462</v>
+        <v>1.392464612725405</v>
       </c>
       <c r="D4" t="n">
-        <v>2.251972007438511</v>
+        <v>2.248701706053477</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -573,7 +573,7 @@
         <v>1.01</v>
       </c>
       <c r="H4" t="n">
-        <v>1.79</v>
+        <v>1.8</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.8454538002499</v>
+        <v>323.9328607341399</v>
       </c>
       <c r="D5" t="n">
-        <v>10.23904542492872</v>
+        <v>10.2513172701727</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.99</v>
+        <v>318.07</v>
       </c>
       <c r="G5" t="n">
-        <v>325.67</v>
+        <v>325.76</v>
       </c>
       <c r="H5" t="n">
-        <v>332.25</v>
+        <v>332.35</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,19 +624,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.03396809739433</v>
+        <v>21.00981532631038</v>
       </c>
       <c r="D6" t="n">
-        <v>2.100131944092435</v>
+        <v>2.124086112344261</v>
       </c>
       <c r="E6" t="n">
-        <v>15.22</v>
+        <v>14.76</v>
       </c>
       <c r="F6" t="n">
-        <v>19.48</v>
+        <v>19.46</v>
       </c>
       <c r="G6" t="n">
-        <v>20.66</v>
+        <v>20.64</v>
       </c>
       <c r="H6" t="n">
         <v>22.2</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.31486173511111</v>
+        <v>-76.33482824130306</v>
       </c>
       <c r="D7" t="n">
-        <v>22.43087720017906</v>
+        <v>22.44113227402011</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.772729262699947</v>
+        <v>7.762797186990312</v>
       </c>
       <c r="D8" t="n">
-        <v>6.826958247165576</v>
+        <v>6.838123600698207</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322383399976859</v>
+        <v>9.322399872309944</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688459844100303</v>
+        <v>1.688394112346986</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8303429706599</v>
+        <v>867.8303629823408</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4610121929352152</v>
+        <v>0.4610342240256628</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569302727017788</v>
+        <v>0.5569113180728144</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5906666965420388</v>
+        <v>0.5906378012529424</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.69027919682621</v>
+        <v>22.6893627954779</v>
       </c>
       <c r="D12" t="n">
-        <v>12.27804715606286</v>
+        <v>12.27781762319351</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6716804562221651</v>
+        <v>0.6716720779220779</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7483016417848986</v>
+        <v>0.7482962772579064</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826072163270429</v>
+        <v>1.825914268585132</v>
       </c>
       <c r="D14" t="n">
-        <v>1.665922424560786</v>
+        <v>1.665830696243136</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.71486173511092</v>
+        <v>93.73482824130286</v>
       </c>
       <c r="D15" t="n">
-        <v>22.43087720014354</v>
+        <v>22.4411322740201</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.63531770634948</v>
+        <v>-85.65015002324094</v>
       </c>
       <c r="D16" t="n">
-        <v>20.23553674694372</v>
+        <v>20.23861619242166</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.0778545523916</v>
+        <v>-101.1469917995764</v>
       </c>
       <c r="G16" t="n">
         <v>-85.69305820175224</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.59612087980607</v>
+        <v>-67.68978441047734</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.86258844364953</v>
+        <v>-77.88735283625061</v>
       </c>
       <c r="D17" t="n">
-        <v>24.79941101361801</v>
+        <v>24.81704205386455</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.22214159641585</v>
+        <v>-92.2376019773414</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.43249407632486</v>
+        <v>-75.41392685158225</v>
       </c>
       <c r="H17" t="n">
-        <v>-56.66683163887967</v>
+        <v>-56.79009749652566</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
More Data, ANOVA moved out of LDPLSM & more .....
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>555.3976844498427</v>
+        <v>552.9146510422127</v>
       </c>
       <c r="D2" t="n">
-        <v>136.1086402776294</v>
+        <v>134.8729807636744</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="G2" t="n">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="H2" t="n">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.65229553045877</v>
+        <v>40.588749505361</v>
       </c>
       <c r="D3" t="n">
-        <v>4.778124445764926</v>
+        <v>4.748913163909507</v>
       </c>
       <c r="E3" t="n">
-        <v>24.86</v>
+        <v>23.23</v>
       </c>
       <c r="F3" t="n">
-        <v>37.68</v>
+        <v>37.66</v>
       </c>
       <c r="G3" t="n">
-        <v>39.94</v>
+        <v>39.9</v>
       </c>
       <c r="H3" t="n">
-        <v>43.32</v>
+        <v>43.17</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.392464612725405</v>
+        <v>1.421047548621008</v>
       </c>
       <c r="D4" t="n">
-        <v>2.248701706053477</v>
+        <v>2.252932184827195</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -570,10 +570,10 @@
         <v>0.51</v>
       </c>
       <c r="G4" t="n">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
       <c r="H4" t="n">
-        <v>1.8</v>
+        <v>1.83</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.9328607341399</v>
+        <v>324.16722179566</v>
       </c>
       <c r="D5" t="n">
-        <v>10.2513172701727</v>
+        <v>10.20123948387039</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>318.07</v>
+        <v>318.37</v>
       </c>
       <c r="G5" t="n">
-        <v>325.76</v>
+        <v>326.13</v>
       </c>
       <c r="H5" t="n">
-        <v>332.35</v>
+        <v>332.5</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.00981532631038</v>
+        <v>20.885195820383</v>
       </c>
       <c r="D6" t="n">
-        <v>2.124086112344261</v>
+        <v>2.246689769048679</v>
       </c>
       <c r="E6" t="n">
-        <v>14.76</v>
+        <v>14.01</v>
       </c>
       <c r="F6" t="n">
-        <v>19.46</v>
+        <v>19.41</v>
       </c>
       <c r="G6" t="n">
-        <v>20.64</v>
+        <v>20.56</v>
       </c>
       <c r="H6" t="n">
-        <v>22.2</v>
+        <v>22.16</v>
       </c>
       <c r="I6" t="n">
-        <v>34.09</v>
+        <v>34.8</v>
       </c>
     </row>
     <row r="7">
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.33482824130306</v>
+        <v>-76.35410958839424</v>
       </c>
       <c r="D7" t="n">
-        <v>22.44113227402011</v>
+        <v>22.44313875632293</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -672,7 +672,7 @@
         <v>-75</v>
       </c>
       <c r="H7" t="n">
-        <v>-56</v>
+        <v>-57</v>
       </c>
       <c r="I7" t="n">
         <v>-32</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.762797186990312</v>
+        <v>7.752670476140048</v>
       </c>
       <c r="D8" t="n">
-        <v>6.838123600698207</v>
+        <v>6.832323163921436</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322399872309944</v>
+        <v>9.322751127871385</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688394112346986</v>
+        <v>1.68816378273026</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8303629823408</v>
+        <v>867.8303584161347</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4610342240256628</v>
+        <v>0.4610671592669811</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569113180728144</v>
+        <v>0.5569279928677539</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5906378012529424</v>
+        <v>0.5905665473748987</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.6893627954779</v>
+        <v>22.68894076892638</v>
       </c>
       <c r="D12" t="n">
-        <v>12.27781762319351</v>
+        <v>12.27785511348378</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6716720779220779</v>
+        <v>0.6716021959611013</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7482962772579064</v>
+        <v>0.7482707418157132</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.825914268585132</v>
+        <v>1.825936178109709</v>
       </c>
       <c r="D14" t="n">
-        <v>1.665830696243136</v>
+        <v>1.665935267887455</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,16 +913,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.73482824130286</v>
+        <v>93.75410958839403</v>
       </c>
       <c r="D15" t="n">
-        <v>22.4411322740201</v>
+        <v>22.44313875632292</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
       </c>
       <c r="F15" t="n">
-        <v>73.40000000000001</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="G15" t="n">
         <v>92.40000000000001</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.65015002324094</v>
+        <v>-85.65962149554009</v>
       </c>
       <c r="D16" t="n">
-        <v>20.23861619242166</v>
+        <v>20.22693921181472</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.1469917995764</v>
+        <v>-101.2123840191425</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.69305820175224</v>
+        <v>-85.5149694202523</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.68978441047734</v>
+        <v>-67.8707776445072</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.88735283625061</v>
+        <v>-77.90695101940007</v>
       </c>
       <c r="D17" t="n">
-        <v>24.81704205386455</v>
+        <v>24.81601411090282</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.2376019773414</v>
+        <v>-92.2778545523916</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.41392685158225</v>
+        <v>-75.3175485570292</v>
       </c>
       <c r="H17" t="n">
-        <v>-56.79009749652566</v>
+        <v>-57.25410721860875</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Genaral Updates, mainly with more data
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>552.9146510422127</v>
+        <v>551.7911908829242</v>
       </c>
       <c r="D2" t="n">
-        <v>134.8729807636744</v>
+        <v>134.8010645558176</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G2" t="n">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H2" t="n">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,10 +525,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.588749505361</v>
+        <v>40.5752808742658</v>
       </c>
       <c r="D3" t="n">
-        <v>4.748913163909507</v>
+        <v>4.739821021780309</v>
       </c>
       <c r="E3" t="n">
         <v>23.23</v>
@@ -537,10 +537,10 @@
         <v>37.66</v>
       </c>
       <c r="G3" t="n">
-        <v>39.9</v>
+        <v>39.89</v>
       </c>
       <c r="H3" t="n">
-        <v>43.17</v>
+        <v>43.15</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.421047548621008</v>
+        <v>1.41712710083542</v>
       </c>
       <c r="D4" t="n">
-        <v>2.252932184827195</v>
+        <v>2.243893152512907</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -573,7 +573,7 @@
         <v>1.03</v>
       </c>
       <c r="H4" t="n">
-        <v>1.83</v>
+        <v>1.82</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>324.16722179566</v>
+        <v>324.0963851543303</v>
       </c>
       <c r="D5" t="n">
-        <v>10.20123948387039</v>
+        <v>10.18603570960344</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>318.37</v>
+        <v>318.16</v>
       </c>
       <c r="G5" t="n">
-        <v>326.13</v>
+        <v>326</v>
       </c>
       <c r="H5" t="n">
-        <v>332.5</v>
+        <v>332.46</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.885195820383</v>
+        <v>20.84400402499239</v>
       </c>
       <c r="D6" t="n">
-        <v>2.246689769048679</v>
+        <v>2.285550540142486</v>
       </c>
       <c r="E6" t="n">
         <v>14.01</v>
       </c>
       <c r="F6" t="n">
-        <v>19.41</v>
+        <v>19.4</v>
       </c>
       <c r="G6" t="n">
-        <v>20.56</v>
+        <v>20.54</v>
       </c>
       <c r="H6" t="n">
-        <v>22.16</v>
+        <v>22.15</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.35410958839424</v>
+        <v>-76.34821987691012</v>
       </c>
       <c r="D7" t="n">
-        <v>22.44313875632293</v>
+        <v>22.43616008784592</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.752670476140048</v>
+        <v>7.75206201747966</v>
       </c>
       <c r="D8" t="n">
-        <v>6.832323163921436</v>
+        <v>6.830867396907287</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322751127871385</v>
+        <v>9.322889570121452</v>
       </c>
       <c r="D9" t="n">
-        <v>1.68816378273026</v>
+        <v>1.688110164882354</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8303584161347</v>
+        <v>867.8303416095284</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4610671592669811</v>
+        <v>0.4610683516698383</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569279928677539</v>
+        <v>0.5569473730409753</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5905665473748987</v>
+        <v>0.5905526589122854</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.68894076892638</v>
+        <v>22.68879601244939</v>
       </c>
       <c r="D12" t="n">
-        <v>12.27785511348378</v>
+        <v>12.27778629887413</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6716021959611013</v>
+        <v>0.6714604638101701</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7482707418157132</v>
+        <v>0.7482366910637375</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.825936178109709</v>
+        <v>1.826063229822386</v>
       </c>
       <c r="D14" t="n">
-        <v>1.665935267887455</v>
+        <v>1.666121582407144</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.75410958839403</v>
+        <v>93.7482198769099</v>
       </c>
       <c r="D15" t="n">
-        <v>22.44313875632292</v>
+        <v>22.43616008784592</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.65962149554009</v>
+        <v>-85.65299769868724</v>
       </c>
       <c r="D16" t="n">
-        <v>20.22693921181472</v>
+        <v>20.21837856105878</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
@@ -958,10 +958,10 @@
         <v>-101.2123840191425</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.5149694202523</v>
+        <v>-85.45410721860875</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.8707776445072</v>
+        <v>-67.95746206410165</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.90695101940007</v>
+        <v>-77.90093568120759</v>
       </c>
       <c r="D17" t="n">
-        <v>24.81601411090282</v>
+        <v>24.80926135014304</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.2778545523916</v>
+        <v>-92.29706163635328</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.3175485570292</v>
+        <v>-75.29706163635328</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.25410721860875</v>
+        <v>-57.26572375596102</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
General Updates based on more data
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>551.7911908829242</v>
+        <v>548.6514879859118</v>
       </c>
       <c r="D2" t="n">
-        <v>134.8010645558176</v>
+        <v>134.4137704555584</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="H2" t="n">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.5752808742658</v>
+        <v>40.53964289067322</v>
       </c>
       <c r="D3" t="n">
-        <v>4.739821021780309</v>
+        <v>4.715725721416273</v>
       </c>
       <c r="E3" t="n">
         <v>23.23</v>
       </c>
       <c r="F3" t="n">
-        <v>37.66</v>
+        <v>37.65</v>
       </c>
       <c r="G3" t="n">
-        <v>39.89</v>
+        <v>39.85</v>
       </c>
       <c r="H3" t="n">
-        <v>43.15</v>
+        <v>43.1</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.41712710083542</v>
+        <v>1.402195413855055</v>
       </c>
       <c r="D4" t="n">
-        <v>2.243893152512907</v>
+        <v>2.218147992283134</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -570,10 +570,10 @@
         <v>0.51</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="H4" t="n">
-        <v>1.82</v>
+        <v>1.8</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>324.0963851543303</v>
+        <v>323.8575897991681</v>
       </c>
       <c r="D5" t="n">
-        <v>10.18603570960344</v>
+        <v>10.27855218193386</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>318.16</v>
+        <v>318</v>
       </c>
       <c r="G5" t="n">
-        <v>326</v>
+        <v>325.63</v>
       </c>
       <c r="H5" t="n">
-        <v>332.46</v>
+        <v>332.36</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.84400402499239</v>
+        <v>20.7228952216187</v>
       </c>
       <c r="D6" t="n">
-        <v>2.285550540142486</v>
+        <v>2.393059563722234</v>
       </c>
       <c r="E6" t="n">
-        <v>14.01</v>
+        <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.4</v>
+        <v>19.34</v>
       </c>
       <c r="G6" t="n">
-        <v>20.54</v>
+        <v>20.45</v>
       </c>
       <c r="H6" t="n">
-        <v>22.15</v>
+        <v>22.12</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.34821987691012</v>
+        <v>-76.45389745753982</v>
       </c>
       <c r="D7" t="n">
-        <v>22.43616008784592</v>
+        <v>22.48866616808437</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.75206201747966</v>
+        <v>7.707435274623196</v>
       </c>
       <c r="D8" t="n">
-        <v>6.830867396907287</v>
+        <v>6.877757018260256</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322889570121452</v>
+        <v>9.32302998759442</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688110164882354</v>
+        <v>1.688001983131599</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8303416095284</v>
+        <v>867.8303149157719</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4610683516698383</v>
+        <v>0.4611064813043405</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569473730409753</v>
+        <v>0.5569493038346092</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5905526589122854</v>
+        <v>0.5905209443196567</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.68879601244939</v>
+        <v>22.68986415844869</v>
       </c>
       <c r="D12" t="n">
-        <v>12.27778629887413</v>
+        <v>12.27851648918861</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6714604638101701</v>
+        <v>0.6713688157821577</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7482366910637375</v>
+        <v>0.7481981734396599</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826063229822386</v>
+        <v>1.826429444519897</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666121582407144</v>
+        <v>1.666535742865267</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.7482198769099</v>
+        <v>93.85389745753963</v>
       </c>
       <c r="D15" t="n">
-        <v>22.43616008784592</v>
+        <v>22.48866616808437</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.65299769868724</v>
+        <v>-85.73525626455496</v>
       </c>
       <c r="D16" t="n">
-        <v>20.21837856105878</v>
+        <v>20.24087520198974</v>
       </c>
       <c r="E16" t="n">
         <v>-137.0738221927363</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.2123840191425</v>
+        <v>-101.4139268515822</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.45410721860875</v>
+        <v>-85.41392685158225</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.95746206410165</v>
+        <v>-68.14699179957641</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.90093568120759</v>
+        <v>-78.02782098993175</v>
       </c>
       <c r="D17" t="n">
-        <v>24.80926135014304</v>
+        <v>24.89145279269826</v>
       </c>
       <c r="E17" t="n">
         <v>-146.0217119216414</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.29706163635328</v>
+        <v>-92.39612087980606</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.29706163635328</v>
+        <v>-75.2778545523916</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.26572375596102</v>
+        <v>-57.3175485570292</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
General - but several updates, and Upgrades
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>548.6514879859118</v>
+        <v>548.4950573743329</v>
       </c>
       <c r="D2" t="n">
-        <v>134.4137704555584</v>
+        <v>134.1831272940331</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
@@ -507,7 +507,7 @@
         <v>503</v>
       </c>
       <c r="H2" t="n">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,10 +525,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.53964289067322</v>
+        <v>40.53816140791415</v>
       </c>
       <c r="D3" t="n">
-        <v>4.715725721416273</v>
+        <v>4.708294320196429</v>
       </c>
       <c r="E3" t="n">
         <v>23.23</v>
@@ -537,10 +537,10 @@
         <v>37.65</v>
       </c>
       <c r="G3" t="n">
-        <v>39.85</v>
+        <v>39.86</v>
       </c>
       <c r="H3" t="n">
-        <v>43.1</v>
+        <v>43.08</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.402195413855055</v>
+        <v>1.390171292267375</v>
       </c>
       <c r="D4" t="n">
-        <v>2.218147992283134</v>
+        <v>2.205551596094132</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -570,10 +570,10 @@
         <v>0.51</v>
       </c>
       <c r="G4" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1.8</v>
+        <v>1.78</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.8575897991681</v>
+        <v>323.5475284446826</v>
       </c>
       <c r="D5" t="n">
-        <v>10.27855218193386</v>
+        <v>10.53104554449298</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>318</v>
+        <v>317.48</v>
       </c>
       <c r="G5" t="n">
-        <v>325.63</v>
+        <v>325.43</v>
       </c>
       <c r="H5" t="n">
-        <v>332.36</v>
+        <v>332.29</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.7228952216187</v>
+        <v>20.68353704656674</v>
       </c>
       <c r="D6" t="n">
-        <v>2.393059563722234</v>
+        <v>2.410231282285922</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.34</v>
+        <v>19.32</v>
       </c>
       <c r="G6" t="n">
-        <v>20.45</v>
+        <v>20.42</v>
       </c>
       <c r="H6" t="n">
-        <v>22.12</v>
+        <v>22.1</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.45389745753982</v>
+        <v>-76.482122217163</v>
       </c>
       <c r="D7" t="n">
-        <v>22.48866616808437</v>
+        <v>22.48240524190338</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.707435274623196</v>
+        <v>7.699387498606519</v>
       </c>
       <c r="D8" t="n">
-        <v>6.877757018260256</v>
+        <v>6.894939634500335</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.32302998759442</v>
+        <v>9.323020592252917</v>
       </c>
       <c r="D9" t="n">
-        <v>1.688001983131599</v>
+        <v>1.687916756027434</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8303149157719</v>
+        <v>867.830306957395</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4611064813043405</v>
+        <v>0.4611338127051571</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569493038346092</v>
+        <v>0.5569145285120393</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5905209443196567</v>
+        <v>0.5904721468873692</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.68986415844869</v>
+        <v>22.68993522093406</v>
       </c>
       <c r="D12" t="n">
-        <v>12.27851648918861</v>
+        <v>12.27851378189118</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6713688157821577</v>
+        <v>0.6713636653473758</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7481981734396599</v>
+        <v>0.7481759703058133</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826429444519897</v>
+        <v>1.826502029229162</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666535742865267</v>
+        <v>1.666587381203018</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.85389745753963</v>
+        <v>93.88212221716277</v>
       </c>
       <c r="D15" t="n">
-        <v>22.48866616808437</v>
+        <v>22.48240524190339</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.73525626455496</v>
+        <v>-85.76217271890657</v>
       </c>
       <c r="D16" t="n">
-        <v>20.24087520198974</v>
+        <v>20.23167260634411</v>
       </c>
       <c r="E16" t="n">
-        <v>-137.0738221927363</v>
+        <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
         <v>-101.4139268515822</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.41392685158225</v>
+        <v>-85.5149694202523</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.14699179957641</v>
+        <v>-68.16954289279533</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.02782098993175</v>
+        <v>-78.06278522030004</v>
       </c>
       <c r="D17" t="n">
-        <v>24.89145279269826</v>
+        <v>24.89797032201137</v>
       </c>
       <c r="E17" t="n">
-        <v>-146.0217119216414</v>
+        <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
         <v>-92.39612087980606</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.2778545523916</v>
+        <v>-75.3175485570292</v>
       </c>
       <c r="H17" t="n">
         <v>-57.3175485570292</v>

</xml_diff>

<commit_message>
Data Sortation & General Upgrades
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>548.4950573743329</v>
+        <v>540.3259683840465</v>
       </c>
       <c r="D2" t="n">
-        <v>134.1831272940331</v>
+        <v>129.5449376653265</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G2" t="n">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="H2" t="n">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.53816140791415</v>
+        <v>41.32955035315693</v>
       </c>
       <c r="D3" t="n">
-        <v>4.708294320196429</v>
+        <v>4.836281502138328</v>
       </c>
       <c r="E3" t="n">
         <v>23.23</v>
       </c>
       <c r="F3" t="n">
-        <v>37.65</v>
+        <v>38.15</v>
       </c>
       <c r="G3" t="n">
-        <v>39.86</v>
+        <v>40.59</v>
       </c>
       <c r="H3" t="n">
-        <v>43.08</v>
+        <v>44.24</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.390171292267375</v>
+        <v>1.429229449054731</v>
       </c>
       <c r="D4" t="n">
-        <v>2.205551596094132</v>
+        <v>2.004718137524667</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="H4" t="n">
-        <v>1.78</v>
+        <v>1.84</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.5475284446826</v>
+        <v>323.0843761917369</v>
       </c>
       <c r="D5" t="n">
-        <v>10.53104554449298</v>
+        <v>10.66518236359977</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.48</v>
+        <v>316.83</v>
       </c>
       <c r="G5" t="n">
-        <v>325.43</v>
+        <v>324.79</v>
       </c>
       <c r="H5" t="n">
-        <v>332.29</v>
+        <v>331.68</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.68353704656674</v>
+        <v>20.80065859962376</v>
       </c>
       <c r="D6" t="n">
-        <v>2.410231282285922</v>
+        <v>2.579163722577207</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.32</v>
+        <v>19.43</v>
       </c>
       <c r="G6" t="n">
-        <v>20.42</v>
+        <v>20.89</v>
       </c>
       <c r="H6" t="n">
-        <v>22.1</v>
+        <v>22.27</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.482122217163</v>
+        <v>-76.29231265034586</v>
       </c>
       <c r="D7" t="n">
-        <v>22.48240524190338</v>
+        <v>22.70534258309803</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,7 +669,7 @@
         <v>-92</v>
       </c>
       <c r="G7" t="n">
-        <v>-75</v>
+        <v>-74</v>
       </c>
       <c r="H7" t="n">
         <v>-57</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.699387498606519</v>
+        <v>7.705900981683519</v>
       </c>
       <c r="D8" t="n">
-        <v>6.894939634500335</v>
+        <v>6.833132541115538</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.323020592252917</v>
+        <v>9.319969256228363</v>
       </c>
       <c r="D9" t="n">
-        <v>1.687916756027434</v>
+        <v>1.684923486802206</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.830306957395</v>
+        <v>867.830103702681</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4611338127051571</v>
+        <v>0.4614640650157109</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5569145285120393</v>
+        <v>0.5549253774386244</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5904721468873692</v>
+        <v>0.5885556454556197</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.68993522093406</v>
+        <v>22.73539255218065</v>
       </c>
       <c r="D12" t="n">
-        <v>12.27851378189118</v>
+        <v>12.29254234512506</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6713636653473758</v>
+        <v>0.6738321139412262</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7481759703058133</v>
+        <v>0.7504700985557685</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826502029229162</v>
+        <v>1.826334777165204</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666587381203018</v>
+        <v>1.664180072947043</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.88212221716277</v>
+        <v>93.69231265034573</v>
       </c>
       <c r="D15" t="n">
-        <v>22.48240524190339</v>
+        <v>22.70534258309803</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -925,7 +925,7 @@
         <v>74.40000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>92.40000000000001</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>109.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.76217271890657</v>
+        <v>-85.56293756301817</v>
       </c>
       <c r="D16" t="n">
-        <v>20.23167260634411</v>
+        <v>20.4547474905328</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.4139268515822</v>
+        <v>-102.0738221927363</v>
       </c>
       <c r="G16" t="n">
-        <v>-85.5149694202523</v>
+        <v>-84.26572375596102</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.16954289279533</v>
+        <v>-67.8707776445072</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.06278522030004</v>
+        <v>-77.85703658133461</v>
       </c>
       <c r="D17" t="n">
-        <v>24.89797032201137</v>
+        <v>25.06701371063542</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.39612087980606</v>
+        <v>-92.71081852649533</v>
       </c>
       <c r="G17" t="n">
-        <v>-75.3175485570292</v>
+        <v>-74.18978441047734</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.3175485570292</v>
+        <v>-57.25410721860875</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
General - but several updates, and Upgrades + more DATA :)
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>540.3259683840465</v>
+        <v>542.020306689403</v>
       </c>
       <c r="D2" t="n">
-        <v>129.5449376653265</v>
+        <v>130.1260856692631</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
@@ -504,10 +504,10 @@
         <v>447</v>
       </c>
       <c r="G2" t="n">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="H2" t="n">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41.32955035315693</v>
+        <v>41.29301825412306</v>
       </c>
       <c r="D3" t="n">
-        <v>4.836281502138328</v>
+        <v>4.826245451811907</v>
       </c>
       <c r="E3" t="n">
         <v>23.23</v>
       </c>
       <c r="F3" t="n">
-        <v>38.15</v>
+        <v>38.13</v>
       </c>
       <c r="G3" t="n">
-        <v>40.59</v>
+        <v>40.57</v>
       </c>
       <c r="H3" t="n">
-        <v>44.24</v>
+        <v>44.16</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.429229449054731</v>
+        <v>1.417583508994922</v>
       </c>
       <c r="D4" t="n">
-        <v>2.004718137524667</v>
+        <v>1.991802455295512</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="G4" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="H4" t="n">
-        <v>1.84</v>
+        <v>1.82</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.0843761917369</v>
+        <v>322.8550222308917</v>
       </c>
       <c r="D5" t="n">
-        <v>10.66518236359977</v>
+        <v>10.7791742118396</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.83</v>
+        <v>316.45</v>
       </c>
       <c r="G5" t="n">
-        <v>324.79</v>
+        <v>324.62</v>
       </c>
       <c r="H5" t="n">
-        <v>331.68</v>
+        <v>331.59</v>
       </c>
       <c r="I5" t="n">
         <v>342.81</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.80065859962376</v>
+        <v>20.77183497668683</v>
       </c>
       <c r="D6" t="n">
-        <v>2.579163722577207</v>
+        <v>2.582807601395347</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.43</v>
+        <v>19.4</v>
       </c>
       <c r="G6" t="n">
-        <v>20.89</v>
+        <v>20.85</v>
       </c>
       <c r="H6" t="n">
-        <v>22.27</v>
+        <v>22.26</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.29231265034586</v>
+        <v>-76.3014969513538</v>
       </c>
       <c r="D7" t="n">
-        <v>22.70534258309803</v>
+        <v>22.74087949442439</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.705900981683519</v>
+        <v>7.687664653310071</v>
       </c>
       <c r="D8" t="n">
-        <v>6.833132541115538</v>
+        <v>6.857906812619937</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.319969256228363</v>
+        <v>9.320027938058054</v>
       </c>
       <c r="D9" t="n">
-        <v>1.684923486802206</v>
+        <v>1.685034460598765</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.830103702681</v>
+        <v>867.8301732285452</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614640650157109</v>
+        <v>0.4614636160985891</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5549253774386244</v>
+        <v>0.5549792477413591</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5885556454556197</v>
+        <v>0.5886060145151576</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.73539255218065</v>
+        <v>22.73730297062099</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29254234512506</v>
+        <v>12.29191041355318</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6738321139412262</v>
+        <v>0.6738143629304758</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7504700985557685</v>
+        <v>0.7504754826094961</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826334777165204</v>
+        <v>1.826669519201123</v>
       </c>
       <c r="D14" t="n">
-        <v>1.664180072947043</v>
+        <v>1.664155219542451</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.69231265034573</v>
+        <v>93.70149695135368</v>
       </c>
       <c r="D15" t="n">
-        <v>22.70534258309803</v>
+        <v>22.74087949442439</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.56293756301817</v>
+        <v>-85.56402711020543</v>
       </c>
       <c r="D16" t="n">
-        <v>20.4547474905328</v>
+        <v>20.48085159011164</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
@@ -961,7 +961,7 @@
         <v>-84.26572375596102</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.8707776445072</v>
+        <v>-67.79706163635328</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.85703658133461</v>
+        <v>-77.87636245689536</v>
       </c>
       <c r="D17" t="n">
-        <v>25.06701371063542</v>
+        <v>25.11899245527042</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.71081852649533</v>
+        <v>-92.79009749652566</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.18978441047734</v>
+        <v>-74.1773721860196</v>
       </c>
       <c r="H17" t="n">
         <v>-57.25410721860875</v>

</xml_diff>

<commit_message>
Data Sortation Plots Update
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>543.4778532294158</v>
+        <v>544.6680519354564</v>
       </c>
       <c r="D2" t="n">
-        <v>131.0485632688492</v>
+        <v>130.9877129156737</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="H2" t="n">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41.25778868341595</v>
+        <v>41.1183126432044</v>
       </c>
       <c r="D3" t="n">
-        <v>4.824759711060782</v>
+        <v>4.88058624883376</v>
       </c>
       <c r="E3" t="n">
-        <v>23.23</v>
+        <v>21.55</v>
       </c>
       <c r="F3" t="n">
-        <v>38.12</v>
+        <v>38.02</v>
       </c>
       <c r="G3" t="n">
-        <v>40.55</v>
+        <v>40.48</v>
       </c>
       <c r="H3" t="n">
-        <v>44.11</v>
+        <v>43.97</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.418564405357841</v>
+        <v>1.434549116830532</v>
       </c>
       <c r="D4" t="n">
-        <v>1.98350376685459</v>
+        <v>1.971442808589984</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="G4" t="n">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
       <c r="H4" t="n">
-        <v>1.82</v>
+        <v>1.86</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,25 +591,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.874941440623</v>
+        <v>323.3270733085213</v>
       </c>
       <c r="D5" t="n">
-        <v>10.72495779235706</v>
+        <v>10.9665986436611</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.6</v>
+        <v>316.93</v>
       </c>
       <c r="G5" t="n">
-        <v>324.6</v>
+        <v>324.9</v>
       </c>
       <c r="H5" t="n">
-        <v>331.53</v>
+        <v>331.95</v>
       </c>
       <c r="I5" t="n">
-        <v>342.81</v>
+        <v>347.57</v>
       </c>
     </row>
     <row r="6">
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.76119199759042</v>
+        <v>20.74015226641773</v>
       </c>
       <c r="D6" t="n">
-        <v>2.581528323953472</v>
+        <v>2.579501233997851</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.39</v>
+        <v>19.36</v>
       </c>
       <c r="G6" t="n">
-        <v>20.84</v>
+        <v>20.8</v>
       </c>
       <c r="H6" t="n">
-        <v>22.25</v>
+        <v>22.24</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.31301076098563</v>
+        <v>-76.26856110659861</v>
       </c>
       <c r="D7" t="n">
-        <v>22.77406728109075</v>
+        <v>22.82112804967369</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,7 +669,7 @@
         <v>-93</v>
       </c>
       <c r="G7" t="n">
-        <v>-74</v>
+        <v>-73</v>
       </c>
       <c r="H7" t="n">
         <v>-57</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.670347249560238</v>
+        <v>7.654260984787354</v>
       </c>
       <c r="D8" t="n">
-        <v>6.876516681297655</v>
+        <v>6.896900002864621</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.32019097451267</v>
+        <v>9.320589911137512</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685068127467219</v>
+        <v>1.685073353967937</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301222963744</v>
+        <v>867.8301002582225</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614419057436024</v>
+        <v>0.4614263505091002</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5550350571255751</v>
+        <v>0.5551466804514653</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5886316502687233</v>
+        <v>0.5886555581242466</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.73813192475524</v>
+        <v>22.73761683659243</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29124422973062</v>
+        <v>12.29076396887385</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6738286257651303</v>
+        <v>0.673866184974602</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7504830367150629</v>
+        <v>0.75047614335641</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826796173539874</v>
+        <v>1.826693903281729</v>
       </c>
       <c r="D14" t="n">
-        <v>1.664030567609022</v>
+        <v>1.663862863133535</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.7130107609855</v>
+        <v>93.66856110659847</v>
       </c>
       <c r="D15" t="n">
-        <v>22.77406728109077</v>
+        <v>22.82112804967369</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -925,7 +925,7 @@
         <v>74.40000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>91.40000000000001</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>110.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.56691460624734</v>
+        <v>-85.51566289683777</v>
       </c>
       <c r="D16" t="n">
-        <v>20.50456927377965</v>
+        <v>20.54218201972368</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.1338080768773</v>
+        <v>-102.1037355585375</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.23249407632485</v>
+        <v>-84.0778545523916</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.8707776445072</v>
+        <v>-67.79706163635328</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.89656735668711</v>
+        <v>-77.86140191205038</v>
       </c>
       <c r="D17" t="n">
-        <v>25.1637078841982</v>
+        <v>25.22542849486244</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.14609373817282</v>
+        <v>-93.01412565612067</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.1773721860196</v>
+        <v>-73.61209675612977</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.25410721860875</v>
+        <v>-57.2376019773414</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Updates with more data
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>544.6680519354564</v>
+        <v>552.5393490234258</v>
       </c>
       <c r="D2" t="n">
-        <v>130.9877129156737</v>
+        <v>135.9824027452931</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="G2" t="n">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="H2" t="n">
-        <v>606</v>
+        <v>621</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41.1183126432044</v>
+        <v>40.34784979735605</v>
       </c>
       <c r="D3" t="n">
-        <v>4.88058624883376</v>
+        <v>5.33264974160819</v>
       </c>
       <c r="E3" t="n">
         <v>21.55</v>
       </c>
       <c r="F3" t="n">
-        <v>38.02</v>
+        <v>37.23</v>
       </c>
       <c r="G3" t="n">
-        <v>40.48</v>
+        <v>40.07</v>
       </c>
       <c r="H3" t="n">
-        <v>43.97</v>
+        <v>43.47</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.434549116830532</v>
+        <v>1.63208194363162</v>
       </c>
       <c r="D4" t="n">
-        <v>1.971442808589984</v>
+        <v>2.160765135266668</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03</v>
+        <v>1.09</v>
       </c>
       <c r="H4" t="n">
-        <v>1.86</v>
+        <v>2.07</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.3270733085213</v>
+        <v>323.4778055602654</v>
       </c>
       <c r="D5" t="n">
-        <v>10.9665986436611</v>
+        <v>11.06650058287537</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.93</v>
+        <v>316.5</v>
       </c>
       <c r="G5" t="n">
-        <v>324.9</v>
+        <v>324.78</v>
       </c>
       <c r="H5" t="n">
-        <v>331.95</v>
+        <v>332.27</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.74015226641773</v>
+        <v>20.78425754650419</v>
       </c>
       <c r="D6" t="n">
-        <v>2.579501233997851</v>
+        <v>2.542140194760566</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.36</v>
+        <v>19.4</v>
       </c>
       <c r="G6" t="n">
         <v>20.8</v>
       </c>
       <c r="H6" t="n">
-        <v>22.24</v>
+        <v>22.26</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.26856110659861</v>
+        <v>-76.08580726674069</v>
       </c>
       <c r="D7" t="n">
-        <v>22.82112804967369</v>
+        <v>22.893064651485</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-93</v>
+        <v>-92</v>
       </c>
       <c r="G7" t="n">
         <v>-73</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.654260984787354</v>
+        <v>7.642853545527799</v>
       </c>
       <c r="D8" t="n">
-        <v>6.896900002864621</v>
+        <v>6.897861818145037</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.320589911137512</v>
+        <v>9.321505417512157</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685073353967937</v>
+        <v>1.685257834954974</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301002582225</v>
+        <v>867.8301581224396</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614263505091002</v>
+        <v>0.4614251634769738</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5551466804514653</v>
+        <v>0.5554575355127357</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5886555581242466</v>
+        <v>0.5887772280295234</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.73761683659243</v>
+        <v>22.74046260795371</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29076396887385</v>
+        <v>12.29178319313078</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.673866184974602</v>
+        <v>0.6738663151619237</v>
       </c>
       <c r="D13" t="n">
-        <v>0.75047614335641</v>
+        <v>0.7505432893694328</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826693903281729</v>
+        <v>1.827044351949593</v>
       </c>
       <c r="D14" t="n">
-        <v>1.663862863133535</v>
+        <v>1.66412783741639</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.66856110659847</v>
+        <v>93.48580726674052</v>
       </c>
       <c r="D15" t="n">
-        <v>22.82112804967369</v>
+        <v>22.893064651485</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -928,7 +928,7 @@
         <v>90.40000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>110.4</v>
+        <v>109.4</v>
       </c>
       <c r="I15" t="n">
         <v>145.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.51566289683777</v>
+        <v>-85.32693461185355</v>
       </c>
       <c r="D16" t="n">
-        <v>20.54218201972368</v>
+        <v>20.60411647482207</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.1037355585375</v>
+        <v>-101.9574620641016</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.0778545523916</v>
+        <v>-83.69305820175224</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.79706163635328</v>
+        <v>-67.69305820175224</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.86140191205038</v>
+        <v>-77.68408106632575</v>
       </c>
       <c r="D17" t="n">
-        <v>25.22542849486244</v>
+        <v>25.30347243440544</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.01412565612067</v>
+        <v>-92.71081852649533</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.61209675612977</v>
+        <v>-72.79009749652566</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.2376019773414</v>
+        <v>-57.21238401914255</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Data Querrying Warnings removed .... ++data
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>552.5393490234258</v>
+        <v>551.0680923226339</v>
       </c>
       <c r="D2" t="n">
-        <v>135.9824027452931</v>
+        <v>135.98277249591</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G2" t="n">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H2" t="n">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.34784979735605</v>
+        <v>40.30310759906428</v>
       </c>
       <c r="D3" t="n">
-        <v>5.33264974160819</v>
+        <v>5.324267421150879</v>
       </c>
       <c r="E3" t="n">
         <v>21.55</v>
       </c>
       <c r="F3" t="n">
-        <v>37.23</v>
+        <v>37.17</v>
       </c>
       <c r="G3" t="n">
-        <v>40.07</v>
+        <v>40.02</v>
       </c>
       <c r="H3" t="n">
-        <v>43.47</v>
+        <v>43.41</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.63208194363162</v>
+        <v>1.620580493539557</v>
       </c>
       <c r="D4" t="n">
-        <v>2.160765135266668</v>
+        <v>2.151637427293199</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -570,10 +570,10 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>1.09</v>
+        <v>1.08</v>
       </c>
       <c r="H4" t="n">
-        <v>2.07</v>
+        <v>2.05</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.4778055602654</v>
+        <v>323.2946474308017</v>
       </c>
       <c r="D5" t="n">
-        <v>11.06650058287537</v>
+        <v>11.14856390329808</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.5</v>
+        <v>315.94</v>
       </c>
       <c r="G5" t="n">
-        <v>324.78</v>
+        <v>324.65</v>
       </c>
       <c r="H5" t="n">
-        <v>332.27</v>
+        <v>332.2</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.78425754650419</v>
+        <v>20.78274570178028</v>
       </c>
       <c r="D6" t="n">
-        <v>2.542140194760566</v>
+        <v>2.53157948035533</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.4</v>
+        <v>19.41</v>
       </c>
       <c r="G6" t="n">
-        <v>20.8</v>
+        <v>20.79</v>
       </c>
       <c r="H6" t="n">
-        <v>22.26</v>
+        <v>22.25</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.08580726674069</v>
+        <v>-76.06973622877116</v>
       </c>
       <c r="D7" t="n">
-        <v>22.893064651485</v>
+        <v>22.89142367125974</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,7 +669,7 @@
         <v>-92</v>
       </c>
       <c r="G7" t="n">
-        <v>-73</v>
+        <v>-72</v>
       </c>
       <c r="H7" t="n">
         <v>-57</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.642853545527799</v>
+        <v>7.644266129774256</v>
       </c>
       <c r="D8" t="n">
-        <v>6.897861818145037</v>
+        <v>6.897221567992845</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.321505417512157</v>
+        <v>9.321485312455726</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685257834954974</v>
+        <v>1.685235526711948</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301581224396</v>
+        <v>867.8301709770533</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614251634769738</v>
+        <v>0.4614231124990945</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5554575355127357</v>
+        <v>0.5554448833875715</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5887772280295234</v>
+        <v>0.5887632158809544</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74046260795371</v>
+        <v>22.73994378273617</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29178319313078</v>
+        <v>12.29186665115116</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6738663151619237</v>
+        <v>0.6738674081548559</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505432893694328</v>
+        <v>0.7505400353874433</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.827044351949593</v>
+        <v>1.826958330223971</v>
       </c>
       <c r="D14" t="n">
-        <v>1.66412783741639</v>
+        <v>1.664121300141535</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.48580726674052</v>
+        <v>93.46973622877101</v>
       </c>
       <c r="D15" t="n">
-        <v>22.893064651485</v>
+        <v>22.89142367125974</v>
       </c>
       <c r="E15" t="n">
         <v>49.4</v>
@@ -925,7 +925,7 @@
         <v>74.40000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>90.40000000000001</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>109.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.32693461185355</v>
+        <v>-85.31226661389034</v>
       </c>
       <c r="D16" t="n">
-        <v>20.60411647482207</v>
+        <v>20.60246642824096</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.9574620641016</v>
+        <v>-101.8707776445072</v>
       </c>
       <c r="G16" t="n">
         <v>-83.69305820175224</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.69305820175224</v>
+        <v>-67.79706163635328</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.68408106632575</v>
+        <v>-77.66800048411609</v>
       </c>
       <c r="D17" t="n">
-        <v>25.30347243440544</v>
+        <v>25.30226435379067</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.71081852649533</v>
+        <v>-92.66683163887967</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.79009749652566</v>
+        <v>-72.71081852649533</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.21238401914255</v>
+        <v>-57.22214159641585</v>
       </c>
       <c r="I17" t="n">
         <v>-33.49305820175223</v>

</xml_diff>

<commit_message>
Updates on all NBs due to ED6; more data analyzed as well...
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>551.0680923226339</v>
+        <v>552.4246960852229</v>
       </c>
       <c r="D2" t="n">
-        <v>135.98277249591</v>
+        <v>136.2986616245581</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="H2" t="n">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.30310759906428</v>
+        <v>40.22822938490521</v>
       </c>
       <c r="D3" t="n">
-        <v>5.324267421150879</v>
+        <v>5.303746036525993</v>
       </c>
       <c r="E3" t="n">
         <v>21.55</v>
       </c>
       <c r="F3" t="n">
-        <v>37.17</v>
+        <v>37.12</v>
       </c>
       <c r="G3" t="n">
-        <v>40.02</v>
+        <v>39.94</v>
       </c>
       <c r="H3" t="n">
-        <v>43.41</v>
+        <v>43.28</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.620580493539557</v>
+        <v>1.599382867147636</v>
       </c>
       <c r="D4" t="n">
-        <v>2.151637427293199</v>
+        <v>2.134985795785292</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="G4" t="n">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="H4" t="n">
-        <v>2.05</v>
+        <v>2.02</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.2946474308017</v>
+        <v>322.8763409526746</v>
       </c>
       <c r="D5" t="n">
-        <v>11.14856390329808</v>
+        <v>11.37829707917052</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>315.94</v>
+        <v>315.06</v>
       </c>
       <c r="G5" t="n">
-        <v>324.65</v>
+        <v>324.32</v>
       </c>
       <c r="H5" t="n">
-        <v>332.2</v>
+        <v>332.05</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.78274570178028</v>
+        <v>20.8051068664887</v>
       </c>
       <c r="D6" t="n">
-        <v>2.53157948035533</v>
+        <v>2.521383329803396</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.41</v>
+        <v>19.44</v>
       </c>
       <c r="G6" t="n">
         <v>20.79</v>
       </c>
       <c r="H6" t="n">
-        <v>22.25</v>
+        <v>22.27</v>
       </c>
       <c r="I6" t="n">
         <v>34.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.06973622877116</v>
+        <v>-76.07091309600243</v>
       </c>
       <c r="D7" t="n">
-        <v>22.89142367125974</v>
+        <v>22.90160120971134</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -675,7 +675,7 @@
         <v>-57</v>
       </c>
       <c r="I7" t="n">
-        <v>-32</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="8">
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.644266129774256</v>
+        <v>7.637385816818627</v>
       </c>
       <c r="D8" t="n">
-        <v>6.897221567992845</v>
+        <v>6.897731999772141</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.321485312455726</v>
+        <v>9.321617443314297</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685235526711948</v>
+        <v>1.685160368922639</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301709770533</v>
+        <v>867.8302478626704</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614231124990945</v>
+        <v>0.4614263994982076</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5554448833875715</v>
+        <v>0.555451883080458</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5887632158809544</v>
+        <v>0.5887337633082016</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.73994378273617</v>
+        <v>22.7386924272632</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29186665115116</v>
+        <v>12.29186826816025</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6738674081548559</v>
+        <v>0.673922042374886</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505400353874433</v>
+        <v>0.7505261244078241</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826958330223971</v>
+        <v>1.826762241070524</v>
       </c>
       <c r="D14" t="n">
-        <v>1.664121300141535</v>
+        <v>1.664037666823125</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,13 +913,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.46973622877101</v>
+        <v>93.47091309600226</v>
       </c>
       <c r="D15" t="n">
-        <v>22.89142367125974</v>
+        <v>22.90160120971134</v>
       </c>
       <c r="E15" t="n">
-        <v>49.4</v>
+        <v>45.4</v>
       </c>
       <c r="F15" t="n">
         <v>74.40000000000001</v>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.31226661389034</v>
+        <v>-85.30844803363917</v>
       </c>
       <c r="D16" t="n">
-        <v>20.60246642824096</v>
+        <v>20.60786016223266</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
@@ -961,7 +961,7 @@
         <v>-83.69305820175224</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.79706163635328</v>
+        <v>-67.8707776445072</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,10 +979,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.66800048411609</v>
+        <v>-77.67106221682054</v>
       </c>
       <c r="D17" t="n">
-        <v>25.30226435379067</v>
+        <v>25.31265400822541</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
@@ -991,13 +991,13 @@
         <v>-92.66683163887967</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.71081852649533</v>
+        <v>-72.75746206410165</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.22214159641585</v>
+        <v>-57.25410721860875</v>
       </c>
       <c r="I17" t="n">
-        <v>-33.49305820175223</v>
+        <v>-28.39612087980607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data fetching concatenation warning handled + more data ....
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>552.4246960852229</v>
+        <v>556.903067169749</v>
       </c>
       <c r="D2" t="n">
-        <v>136.2986616245581</v>
+        <v>137.0797485771566</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="G2" t="n">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="H2" t="n">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40.22822938490521</v>
+        <v>39.7527068601508</v>
       </c>
       <c r="D3" t="n">
-        <v>5.303746036525993</v>
+        <v>5.498549166859621</v>
       </c>
       <c r="E3" t="n">
-        <v>21.55</v>
+        <v>19.17</v>
       </c>
       <c r="F3" t="n">
-        <v>37.12</v>
+        <v>36.56</v>
       </c>
       <c r="G3" t="n">
-        <v>39.94</v>
+        <v>39.55</v>
       </c>
       <c r="H3" t="n">
-        <v>43.28</v>
+        <v>42.89</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.599382867147636</v>
+        <v>1.699852359697954</v>
       </c>
       <c r="D4" t="n">
-        <v>2.134985795785292</v>
+        <v>2.200329288054807</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.55</v>
+        <v>0.57</v>
       </c>
       <c r="G4" t="n">
-        <v>1.06</v>
+        <v>1.11</v>
       </c>
       <c r="H4" t="n">
-        <v>2.02</v>
+        <v>2.14</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.8763409526746</v>
+        <v>323.5643501279831</v>
       </c>
       <c r="D5" t="n">
-        <v>11.37829707917052</v>
+        <v>11.37798183850485</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>315.06</v>
+        <v>316.09</v>
       </c>
       <c r="G5" t="n">
-        <v>324.32</v>
+        <v>325.18</v>
       </c>
       <c r="H5" t="n">
-        <v>332.05</v>
+        <v>332.46</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.8051068664887</v>
+        <v>20.86686181265001</v>
       </c>
       <c r="D6" t="n">
-        <v>2.521383329803396</v>
+        <v>2.527131286839315</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.44</v>
+        <v>19.48</v>
       </c>
       <c r="G6" t="n">
-        <v>20.79</v>
+        <v>20.81</v>
       </c>
       <c r="H6" t="n">
-        <v>22.27</v>
+        <v>22.31</v>
       </c>
       <c r="I6" t="n">
-        <v>34.8</v>
+        <v>37.8</v>
       </c>
     </row>
     <row r="7">
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.07091309600243</v>
+        <v>-76.24924404900628</v>
       </c>
       <c r="D7" t="n">
-        <v>22.90160120971134</v>
+        <v>23.01777259675368</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-92</v>
+        <v>-93</v>
       </c>
       <c r="G7" t="n">
         <v>-72</v>
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.637385816818627</v>
+        <v>7.557583971088439</v>
       </c>
       <c r="D8" t="n">
-        <v>6.897731999772141</v>
+        <v>6.967010693220619</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="G8" t="n">
         <v>9.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.321617443314297</v>
+        <v>9.322028731546192</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685160368922639</v>
+        <v>1.685296913919198</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8302478626704</v>
+        <v>867.8301435397293</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614263994982076</v>
+        <v>0.461476958793068</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.555451883080458</v>
+        <v>0.555614872938282</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5887337633082016</v>
+        <v>0.5888382736154281</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.7386924272632</v>
+        <v>22.73680810202462</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29186826816025</v>
+        <v>12.29101085861106</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.673922042374886</v>
+        <v>0.6739719803998502</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505261244078241</v>
+        <v>0.7505078519842362</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826762241070524</v>
+        <v>1.826418901577393</v>
       </c>
       <c r="D14" t="n">
-        <v>1.664037666823125</v>
+        <v>1.663703329637374</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.47091309600226</v>
+        <v>93.64924404900609</v>
       </c>
       <c r="D15" t="n">
-        <v>22.90160120971134</v>
+        <v>23.01777259675369</v>
       </c>
       <c r="E15" t="n">
         <v>45.4</v>
@@ -928,7 +928,7 @@
         <v>89.40000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>109.4</v>
+        <v>110.4</v>
       </c>
       <c r="I15" t="n">
         <v>145.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.30844803363917</v>
+        <v>-85.44001163749608</v>
       </c>
       <c r="D16" t="n">
-        <v>20.60786016223266</v>
+        <v>20.67387923932912</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.8707776445072</v>
+        <v>-102.265723755961</v>
       </c>
       <c r="G16" t="n">
-        <v>-83.69305820175224</v>
+        <v>-83.5175485570292</v>
       </c>
       <c r="H16" t="n">
-        <v>-67.8707776445072</v>
+        <v>-68.7376019773414</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.67106221682054</v>
+        <v>-77.88242766640762</v>
       </c>
       <c r="D17" t="n">
-        <v>25.31265400822541</v>
+        <v>25.46912265037626</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.66683163887967</v>
+        <v>-93.39612087980606</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.75746206410165</v>
+        <v>-72.61209675612977</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.25410721860875</v>
+        <v>-57.69982180459142</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
Ensured sorted data based on time after anomaly detection per device + More data
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>556.903067169749</v>
+        <v>556.0118747503398</v>
       </c>
       <c r="D2" t="n">
-        <v>137.0797485771566</v>
+        <v>136.9457962890611</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G2" t="n">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H2" t="n">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>39.7527068601508</v>
+        <v>39.52368681086599</v>
       </c>
       <c r="D3" t="n">
-        <v>5.498549166859621</v>
+        <v>5.606686868718929</v>
       </c>
       <c r="E3" t="n">
         <v>19.17</v>
       </c>
       <c r="F3" t="n">
-        <v>36.56</v>
+        <v>36.2</v>
       </c>
       <c r="G3" t="n">
-        <v>39.55</v>
+        <v>39.38</v>
       </c>
       <c r="H3" t="n">
-        <v>42.89</v>
+        <v>42.73</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.699852359697954</v>
+        <v>1.871659445233377</v>
       </c>
       <c r="D4" t="n">
-        <v>2.200329288054807</v>
+        <v>2.547662974226376</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
       <c r="G4" t="n">
-        <v>1.11</v>
+        <v>1.14</v>
       </c>
       <c r="H4" t="n">
-        <v>2.14</v>
+        <v>2.27</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.5643501279831</v>
+        <v>323.6522252399128</v>
       </c>
       <c r="D5" t="n">
-        <v>11.37798183850485</v>
+        <v>11.24365883105295</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.09</v>
+        <v>316.56</v>
       </c>
       <c r="G5" t="n">
-        <v>325.18</v>
+        <v>325.26</v>
       </c>
       <c r="H5" t="n">
-        <v>332.46</v>
+        <v>332.32</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.86686181265001</v>
+        <v>20.85940448499746</v>
       </c>
       <c r="D6" t="n">
-        <v>2.527131286839315</v>
+        <v>2.514335804458083</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.48</v>
+        <v>19.45</v>
       </c>
       <c r="G6" t="n">
-        <v>20.81</v>
+        <v>20.79</v>
       </c>
       <c r="H6" t="n">
-        <v>22.31</v>
+        <v>22.29</v>
       </c>
       <c r="I6" t="n">
         <v>37.8</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.24924404900628</v>
+        <v>-76.34696996049395</v>
       </c>
       <c r="D7" t="n">
-        <v>23.01777259675368</v>
+        <v>23.05853417398344</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -672,7 +672,7 @@
         <v>-72</v>
       </c>
       <c r="H7" t="n">
-        <v>-57</v>
+        <v>-58</v>
       </c>
       <c r="I7" t="n">
         <v>-28</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.557583971088439</v>
+        <v>7.530281690140845</v>
       </c>
       <c r="D8" t="n">
-        <v>6.967010693220619</v>
+        <v>6.973085129280163</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322028731546192</v>
+        <v>9.321963796632716</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685296913919198</v>
+        <v>1.685559257197546</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301435397293</v>
+        <v>867.8300477245315</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461476958793068</v>
+        <v>0.4614970413315863</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.555614872938282</v>
+        <v>0.5556898985686461</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5888382736154281</v>
+        <v>0.5889505257655291</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.73680810202462</v>
+        <v>22.7405931832473</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29101085861106</v>
+        <v>12.2918382459891</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6739719803998502</v>
+        <v>0.6741066223760586</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505078519842362</v>
+        <v>0.7505689471373156</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826418901577393</v>
+        <v>1.826884373608353</v>
       </c>
       <c r="D14" t="n">
-        <v>1.663703329637374</v>
+        <v>1.663848617717044</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,16 +913,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.64924404900609</v>
+        <v>93.74696996049376</v>
       </c>
       <c r="D15" t="n">
-        <v>23.01777259675369</v>
+        <v>23.05853417398344</v>
       </c>
       <c r="E15" t="n">
         <v>45.4</v>
       </c>
       <c r="F15" t="n">
-        <v>74.40000000000001</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="G15" t="n">
         <v>89.40000000000001</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.44001163749608</v>
+        <v>-85.51812118107686</v>
       </c>
       <c r="D16" t="n">
-        <v>20.67387923932912</v>
+        <v>20.69690774443287</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.265723755961</v>
+        <v>-102.4668316388797</v>
       </c>
       <c r="G16" t="n">
         <v>-83.5175485570292</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.7376019773414</v>
+        <v>-68.8707776445072</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.88242766640762</v>
+        <v>-77.98783949093604</v>
       </c>
       <c r="D17" t="n">
-        <v>25.46912265037626</v>
+        <v>25.51063393418753</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.39612087980606</v>
+        <v>-93.53779541063678</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.61209675612977</v>
+        <v>-72.57382219273629</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.69982180459142</v>
+        <v>-58.22214159641585</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
Main update is new / more data ....
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>556.0118747503398</v>
+        <v>554.2244097746863</v>
       </c>
       <c r="D2" t="n">
-        <v>136.9457962890611</v>
+        <v>137.036859118281</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H2" t="n">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>39.52368681086599</v>
+        <v>38.04572514902715</v>
       </c>
       <c r="D3" t="n">
-        <v>5.606686868718929</v>
+        <v>6.407910327843007</v>
       </c>
       <c r="E3" t="n">
-        <v>19.17</v>
+        <v>13.99</v>
       </c>
       <c r="F3" t="n">
-        <v>36.2</v>
+        <v>33.55</v>
       </c>
       <c r="G3" t="n">
-        <v>39.38</v>
+        <v>38.32</v>
       </c>
       <c r="H3" t="n">
-        <v>42.73</v>
+        <v>41.93</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.871659445233377</v>
+        <v>1.985393321247786</v>
       </c>
       <c r="D4" t="n">
-        <v>2.547662974226376</v>
+        <v>2.578404066613742</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.58</v>
+        <v>0.62</v>
       </c>
       <c r="G4" t="n">
-        <v>1.14</v>
+        <v>1.25</v>
       </c>
       <c r="H4" t="n">
-        <v>2.27</v>
+        <v>2.44</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.6522252399128</v>
+        <v>323.4510987676962</v>
       </c>
       <c r="D5" t="n">
-        <v>11.24365883105295</v>
+        <v>11.06316211009865</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.56</v>
+        <v>316.47</v>
       </c>
       <c r="G5" t="n">
-        <v>325.26</v>
+        <v>325.1</v>
       </c>
       <c r="H5" t="n">
-        <v>332.32</v>
+        <v>331.91</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.85940448499746</v>
+        <v>21.07518195672249</v>
       </c>
       <c r="D6" t="n">
-        <v>2.514335804458083</v>
+        <v>2.570000824648706</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.45</v>
+        <v>19.61</v>
       </c>
       <c r="G6" t="n">
-        <v>20.79</v>
+        <v>20.97</v>
       </c>
       <c r="H6" t="n">
-        <v>22.29</v>
+        <v>22.42</v>
       </c>
       <c r="I6" t="n">
-        <v>37.8</v>
+        <v>40.24</v>
       </c>
     </row>
     <row r="7">
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.34696996049395</v>
+        <v>-76.82220451406528</v>
       </c>
       <c r="D7" t="n">
-        <v>23.05853417398344</v>
+        <v>23.0079584737104</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,10 +669,10 @@
         <v>-93</v>
       </c>
       <c r="G7" t="n">
-        <v>-72</v>
+        <v>-73</v>
       </c>
       <c r="H7" t="n">
-        <v>-58</v>
+        <v>-60</v>
       </c>
       <c r="I7" t="n">
         <v>-28</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.530281690140845</v>
+        <v>7.423295699108116</v>
       </c>
       <c r="D8" t="n">
-        <v>6.973085129280163</v>
+        <v>7.085579705271992</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.321963796632716</v>
+        <v>9.323212364260757</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685559257197546</v>
+        <v>1.685514881819898</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8300477245315</v>
+        <v>867.8301860059754</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614970413315863</v>
+        <v>0.4614917528972468</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5556898985686461</v>
+        <v>0.5560061666279863</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5889505257655291</v>
+        <v>0.5889881137317596</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.7405931832473</v>
+        <v>22.74361573155155</v>
       </c>
       <c r="D12" t="n">
-        <v>12.2918382459891</v>
+        <v>12.2924745200119</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6741066223760586</v>
+        <v>0.6739831830213758</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505689471373156</v>
+        <v>0.7505851136300418</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.826884373608353</v>
+        <v>1.827398756497875</v>
       </c>
       <c r="D14" t="n">
-        <v>1.663848617717044</v>
+        <v>1.66421572398068</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,19 +913,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.74696996049376</v>
+        <v>94.22220451406506</v>
       </c>
       <c r="D15" t="n">
-        <v>23.05853417398344</v>
+        <v>23.00795847371041</v>
       </c>
       <c r="E15" t="n">
         <v>45.4</v>
       </c>
       <c r="F15" t="n">
-        <v>75.40000000000001</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>89.40000000000001</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>110.4</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.51812118107686</v>
+        <v>-85.941394822696</v>
       </c>
       <c r="D16" t="n">
-        <v>20.69690774443287</v>
+        <v>20.58142603228347</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.4668316388797</v>
+        <v>-102.8120967561298</v>
       </c>
       <c r="G16" t="n">
-        <v>-83.5175485570292</v>
+        <v>-84.0778545523916</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.8707776445072</v>
+        <v>-70.02214159641585</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.98783949093604</v>
+        <v>-78.51809912358789</v>
       </c>
       <c r="D17" t="n">
-        <v>25.51063393418753</v>
+        <v>25.53711788267815</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.53779541063678</v>
+        <v>-94.22214159641585</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.57382219273629</v>
+        <v>-73.46183611348224</v>
       </c>
       <c r="H17" t="n">
-        <v>-58.22214159641585</v>
+        <v>-60.18978441047734</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
Updated Link Budget Analysis: Antenna Gains and Cable losses
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -913,25 +913,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>94.22220451406506</v>
+        <v>94.08220451406545</v>
       </c>
       <c r="D15" t="n">
-        <v>23.00795847371041</v>
+        <v>23.00795847371039</v>
       </c>
       <c r="E15" t="n">
-        <v>45.4</v>
+        <v>45.26</v>
       </c>
       <c r="F15" t="n">
-        <v>77.40000000000001</v>
+        <v>77.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>90.40000000000001</v>
+        <v>90.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>110.4</v>
+        <v>110.26</v>
       </c>
       <c r="I15" t="n">
-        <v>145.4</v>
+        <v>145.26</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
Makdown cells enrichment for Data Querying and Sorting. Sorting code made precise too!
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>554.2244097746863</v>
+        <v>554.5640449799788</v>
       </c>
       <c r="D2" t="n">
-        <v>137.036859118281</v>
+        <v>136.2932116927976</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
@@ -504,7 +504,7 @@
         <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="H2" t="n">
         <v>625</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>38.04572514902715</v>
+        <v>37.64364162057874</v>
       </c>
       <c r="D3" t="n">
-        <v>6.407910327843007</v>
+        <v>6.502298985304678</v>
       </c>
       <c r="E3" t="n">
         <v>13.99</v>
       </c>
       <c r="F3" t="n">
-        <v>33.55</v>
+        <v>32.95</v>
       </c>
       <c r="G3" t="n">
-        <v>38.32</v>
+        <v>37.95</v>
       </c>
       <c r="H3" t="n">
-        <v>41.93</v>
+        <v>41.59</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,19 +558,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.985393321247786</v>
+        <v>2.002309828873187</v>
       </c>
       <c r="D4" t="n">
-        <v>2.578404066613742</v>
+        <v>2.559219627636518</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="G4" t="n">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
       <c r="H4" t="n">
         <v>2.44</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.4510987676962</v>
+        <v>323.2802032006397</v>
       </c>
       <c r="D5" t="n">
-        <v>11.06316211009865</v>
+        <v>10.88097831185358</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.47</v>
+        <v>316.25</v>
       </c>
       <c r="G5" t="n">
-        <v>325.1</v>
+        <v>324.79</v>
       </c>
       <c r="H5" t="n">
-        <v>331.91</v>
+        <v>331.56</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.07518195672249</v>
+        <v>21.18694478796489</v>
       </c>
       <c r="D6" t="n">
-        <v>2.570000824648706</v>
+        <v>2.589795419055544</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.61</v>
+        <v>19.71</v>
       </c>
       <c r="G6" t="n">
-        <v>20.97</v>
+        <v>21.13</v>
       </c>
       <c r="H6" t="n">
-        <v>22.42</v>
+        <v>22.52</v>
       </c>
       <c r="I6" t="n">
         <v>40.24</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.82220451406528</v>
+        <v>-76.88942345266391</v>
       </c>
       <c r="D7" t="n">
-        <v>23.0079584737104</v>
+        <v>22.93711828158775</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.423295699108116</v>
+        <v>7.415725274312365</v>
       </c>
       <c r="D8" t="n">
-        <v>7.085579705271992</v>
+        <v>7.102650580236241</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.323212364260757</v>
+        <v>9.322666065952859</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685514881819898</v>
+        <v>1.685729385373283</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301860059754</v>
+        <v>867.8300902449899</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614917528972468</v>
+        <v>0.4614888068895844</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5560061666279863</v>
+        <v>0.555930376485119</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5889881137317596</v>
+        <v>0.5890373160311491</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74361573155155</v>
+        <v>22.74735387100284</v>
       </c>
       <c r="D12" t="n">
-        <v>12.2924745200119</v>
+        <v>12.29392615808524</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6739831830213758</v>
+        <v>0.6740300081065715</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505851136300418</v>
+        <v>0.7506847753406487</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.827398756497875</v>
+        <v>1.827769834665784</v>
       </c>
       <c r="D14" t="n">
-        <v>1.66421572398068</v>
+        <v>1.66448662828912</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>94.08220451406545</v>
+        <v>94.14942345266408</v>
       </c>
       <c r="D15" t="n">
-        <v>23.00795847371039</v>
+        <v>22.93711828158775</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.941394822696</v>
+        <v>-86.00904533313746</v>
       </c>
       <c r="D16" t="n">
-        <v>20.58142603228347</v>
+        <v>20.50881087638902</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.8120967561298</v>
+        <v>-102.7900974965257</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.0778545523916</v>
+        <v>-84.26572375596102</v>
       </c>
       <c r="H16" t="n">
-        <v>-70.02214159641585</v>
+        <v>-70.33779541063677</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.51809912358789</v>
+        <v>-78.59332005882511</v>
       </c>
       <c r="D17" t="n">
-        <v>25.53711788267815</v>
+        <v>25.48295048108626</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-94.22214159641585</v>
+        <v>-93.93380807687734</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.46183611348224</v>
+        <v>-73.71081852649533</v>
       </c>
       <c r="H17" t="n">
-        <v>-60.18978441047734</v>
+        <v>-60.33195619988427</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
EDA up to 1st April 2025
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>554.5640449799788</v>
+        <v>553.9339164698035</v>
       </c>
       <c r="D2" t="n">
-        <v>136.2932116927976</v>
+        <v>136.0796753216453</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
@@ -504,7 +504,7 @@
         <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H2" t="n">
         <v>625</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.64364162057874</v>
+        <v>37.54371199562761</v>
       </c>
       <c r="D3" t="n">
-        <v>6.502298985304678</v>
+        <v>6.493415194419221</v>
       </c>
       <c r="E3" t="n">
         <v>13.99</v>
       </c>
       <c r="F3" t="n">
-        <v>32.95</v>
+        <v>32.81</v>
       </c>
       <c r="G3" t="n">
-        <v>37.95</v>
+        <v>37.81</v>
       </c>
       <c r="H3" t="n">
-        <v>41.59</v>
+        <v>41.51</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.002309828873187</v>
+        <v>1.98216252087201</v>
       </c>
       <c r="D4" t="n">
-        <v>2.559219627636518</v>
+        <v>2.542316588930305</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -570,10 +570,10 @@
         <v>0.63</v>
       </c>
       <c r="G4" t="n">
-        <v>1.29</v>
+        <v>1.27</v>
       </c>
       <c r="H4" t="n">
-        <v>2.44</v>
+        <v>2.41</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.2802032006397</v>
+        <v>323.3209024386936</v>
       </c>
       <c r="D5" t="n">
-        <v>10.88097831185358</v>
+        <v>10.80527007418991</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.25</v>
+        <v>316.54</v>
       </c>
       <c r="G5" t="n">
-        <v>324.79</v>
+        <v>324.78</v>
       </c>
       <c r="H5" t="n">
-        <v>331.56</v>
+        <v>331.49</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.18694478796489</v>
+        <v>21.20733341915513</v>
       </c>
       <c r="D6" t="n">
-        <v>2.589795419055544</v>
+        <v>2.579251734900613</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.71</v>
+        <v>19.73</v>
       </c>
       <c r="G6" t="n">
-        <v>21.13</v>
+        <v>21.17</v>
       </c>
       <c r="H6" t="n">
-        <v>22.52</v>
+        <v>22.53</v>
       </c>
       <c r="I6" t="n">
         <v>40.24</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.88942345266391</v>
+        <v>-76.90280080160562</v>
       </c>
       <c r="D7" t="n">
-        <v>22.93711828158775</v>
+        <v>22.89926493007523</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.415725274312365</v>
+        <v>7.419475878633727</v>
       </c>
       <c r="D8" t="n">
-        <v>7.102650580236241</v>
+        <v>7.098372356560299</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322666065952859</v>
+        <v>9.322680892004572</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685729385373283</v>
+        <v>1.685704350771354</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8300902449899</v>
+        <v>867.8301139623015</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614888068895844</v>
+        <v>0.461504525285086</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.555930376485119</v>
+        <v>0.5559225975394744</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5890373160311491</v>
+        <v>0.5890156371207561</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74735387100284</v>
+        <v>22.74623852133575</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29392615808524</v>
+        <v>12.29406113203675</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6740300081065715</v>
+        <v>0.6740255086446632</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7506847753406487</v>
+        <v>0.7506961663209128</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.827769834665784</v>
+        <v>1.827532081539733</v>
       </c>
       <c r="D14" t="n">
-        <v>1.66448662828912</v>
+        <v>1.664426921769673</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>94.14942345266408</v>
+        <v>94.1628008016058</v>
       </c>
       <c r="D15" t="n">
-        <v>22.93711828158775</v>
+        <v>22.89926493007523</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-86.00904533313746</v>
+        <v>-86.02480107908279</v>
       </c>
       <c r="D16" t="n">
-        <v>20.50881087638902</v>
+        <v>20.47195713111128</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.7900974965257</v>
+        <v>-102.7376019773414</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.26572375596102</v>
+        <v>-84.23249407632485</v>
       </c>
       <c r="H16" t="n">
-        <v>-70.33779541063677</v>
+        <v>-70.46683163887967</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.59332005882511</v>
+        <v>-78.60532520044909</v>
       </c>
       <c r="D17" t="n">
-        <v>25.48295048108626</v>
+        <v>25.44454038663014</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.93380807687734</v>
+        <v>-93.87736039420676</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.71081852649533</v>
+        <v>-73.57382219273629</v>
       </c>
       <c r="H17" t="n">
-        <v>-60.33195619988427</v>
+        <v>-60.41392685158225</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
EDA with 1.7 M rows by May 22, 2025
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>553.9339164698035</v>
+        <v>542.0609781685043</v>
       </c>
       <c r="D2" t="n">
-        <v>136.0796753216453</v>
+        <v>132.8868025705442</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="G2" t="n">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="H2" t="n">
-        <v>625</v>
+        <v>603</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.54371199562761</v>
+        <v>36.13728657786727</v>
       </c>
       <c r="D3" t="n">
-        <v>6.493415194419221</v>
+        <v>6.670571437050095</v>
       </c>
       <c r="E3" t="n">
-        <v>13.99</v>
+        <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.81</v>
+        <v>31.13</v>
       </c>
       <c r="G3" t="n">
-        <v>37.81</v>
+        <v>36.16</v>
       </c>
       <c r="H3" t="n">
-        <v>41.51</v>
+        <v>40.52</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.98216252087201</v>
+        <v>1.898863786573787</v>
       </c>
       <c r="D4" t="n">
-        <v>2.542316588930305</v>
+        <v>2.333213627382802</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="G4" t="n">
         <v>1.27</v>
       </c>
       <c r="H4" t="n">
-        <v>2.41</v>
+        <v>2.35</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.3209024386936</v>
+        <v>322.9634159664012</v>
       </c>
       <c r="D5" t="n">
-        <v>10.80527007418991</v>
+        <v>9.912160637139898</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.54</v>
+        <v>317.29</v>
       </c>
       <c r="G5" t="n">
-        <v>324.78</v>
+        <v>323.82</v>
       </c>
       <c r="H5" t="n">
-        <v>331.49</v>
+        <v>330.28</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.20733341915513</v>
+        <v>21.95410935447361</v>
       </c>
       <c r="D6" t="n">
-        <v>2.579251734900613</v>
+        <v>2.898002914381816</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.73</v>
+        <v>20.18</v>
       </c>
       <c r="G6" t="n">
-        <v>21.17</v>
+        <v>21.86</v>
       </c>
       <c r="H6" t="n">
-        <v>22.53</v>
+        <v>23.54</v>
       </c>
       <c r="I6" t="n">
-        <v>40.24</v>
+        <v>43.95</v>
       </c>
     </row>
     <row r="7">
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.90280080160562</v>
+        <v>-76.65418777953791</v>
       </c>
       <c r="D7" t="n">
-        <v>22.89926493007523</v>
+        <v>22.63935614326323</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-93</v>
+        <v>-92</v>
       </c>
       <c r="G7" t="n">
         <v>-73</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.419475878633727</v>
+        <v>7.469847364979513</v>
       </c>
       <c r="D8" t="n">
-        <v>7.098372356560299</v>
+        <v>7.066212116931776</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -708,7 +708,7 @@
         <v>11.2</v>
       </c>
       <c r="I8" t="n">
-        <v>19</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322680892004572</v>
+        <v>9.323211394481104</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685704350771354</v>
+        <v>1.684983442039149</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301139623015</v>
+        <v>867.8302414414916</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461504525285086</v>
+        <v>0.4616029512748378</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5559225975394744</v>
+        <v>0.555803060880837</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5890156371207561</v>
+        <v>0.5886708498917116</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74623852133575</v>
+        <v>22.74662339766567</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29406113203675</v>
+        <v>12.29661590163144</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6740255086446632</v>
+        <v>0.6736168665176964</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7506961663209128</v>
+        <v>0.7503719671250473</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.827532081539733</v>
+        <v>1.829012261493037</v>
       </c>
       <c r="D14" t="n">
-        <v>1.664426921769673</v>
+        <v>1.666376028037912</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>94.1628008016058</v>
+        <v>93.91418777953784</v>
       </c>
       <c r="D15" t="n">
-        <v>22.89926493007523</v>
+        <v>22.63935614324561</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -928,7 +928,7 @@
         <v>90.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>110.26</v>
+        <v>109.26</v>
       </c>
       <c r="I15" t="n">
         <v>145.26</v>
@@ -946,19 +946,19 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-86.02480107908279</v>
+        <v>-85.80869979240862</v>
       </c>
       <c r="D16" t="n">
-        <v>20.47195713111128</v>
+        <v>20.23570194439699</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.7376019773414</v>
+        <v>-101.9574620641016</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.23249407632485</v>
+        <v>-84.0778545523916</v>
       </c>
       <c r="H16" t="n">
         <v>-70.46683163887967</v>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.60532520044909</v>
+        <v>-78.33885242742906</v>
       </c>
       <c r="D17" t="n">
-        <v>25.44454038663014</v>
+        <v>25.18574384850274</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.87736039420676</v>
+        <v>-93.2376019773414</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.57382219273629</v>
+        <v>-73.49305820175223</v>
       </c>
       <c r="H17" t="n">
         <v>-60.41392685158225</v>

</xml_diff>

<commit_message>
In preparation for the EuCNC and 6G Summit
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>542.0609781685043</v>
+        <v>553.9339164698035</v>
       </c>
       <c r="D2" t="n">
-        <v>132.8868025705442</v>
+        <v>136.0796753216788</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="G2" t="n">
-        <v>496</v>
+        <v>513</v>
       </c>
       <c r="H2" t="n">
-        <v>603</v>
+        <v>625</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36.13728657786727</v>
+        <v>37.54371199562761</v>
       </c>
       <c r="D3" t="n">
-        <v>6.670571437050095</v>
+        <v>6.49341519441723</v>
       </c>
       <c r="E3" t="n">
-        <v>13.96</v>
+        <v>13.99</v>
       </c>
       <c r="F3" t="n">
-        <v>31.13</v>
+        <v>32.81</v>
       </c>
       <c r="G3" t="n">
-        <v>36.16</v>
+        <v>37.81</v>
       </c>
       <c r="H3" t="n">
-        <v>40.52</v>
+        <v>41.51</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.898863786573787</v>
+        <v>1.98216252087201</v>
       </c>
       <c r="D4" t="n">
-        <v>2.333213627382802</v>
+        <v>2.542316588933395</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="G4" t="n">
         <v>1.27</v>
       </c>
       <c r="H4" t="n">
-        <v>2.35</v>
+        <v>2.41</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.9634159664012</v>
+        <v>323.3209024386936</v>
       </c>
       <c r="D5" t="n">
-        <v>9.912160637139898</v>
+        <v>10.80527007418962</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.29</v>
+        <v>316.54</v>
       </c>
       <c r="G5" t="n">
-        <v>323.82</v>
+        <v>324.78</v>
       </c>
       <c r="H5" t="n">
-        <v>330.28</v>
+        <v>331.49</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.95410935447361</v>
+        <v>21.20733341915513</v>
       </c>
       <c r="D6" t="n">
-        <v>2.898002914381816</v>
+        <v>2.579251734899544</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>20.18</v>
+        <v>19.73</v>
       </c>
       <c r="G6" t="n">
-        <v>21.86</v>
+        <v>21.17</v>
       </c>
       <c r="H6" t="n">
-        <v>23.54</v>
+        <v>22.53</v>
       </c>
       <c r="I6" t="n">
-        <v>43.95</v>
+        <v>40.24</v>
       </c>
     </row>
     <row r="7">
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.65418777953791</v>
+        <v>-76.90280080160562</v>
       </c>
       <c r="D7" t="n">
-        <v>22.63935614326323</v>
+        <v>22.89926493012658</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-92</v>
+        <v>-93</v>
       </c>
       <c r="G7" t="n">
         <v>-73</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.469847364979513</v>
+        <v>7.419475878633727</v>
       </c>
       <c r="D8" t="n">
-        <v>7.066212116931776</v>
+        <v>7.098372356541219</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -708,7 +708,7 @@
         <v>11.2</v>
       </c>
       <c r="I8" t="n">
-        <v>25.2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.323211394481104</v>
+        <v>9.322680892004572</v>
       </c>
       <c r="D9" t="n">
-        <v>1.684983442039149</v>
+        <v>1.685704350766166</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8302414414916</v>
+        <v>867.8301139623015</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4616029512748378</v>
+        <v>0.461504525281789</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.555803060880837</v>
+        <v>0.5559225975394744</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5886708498917116</v>
+        <v>0.5890156371236127</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74662339766567</v>
+        <v>22.74623852133575</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29661590163144</v>
+        <v>12.29406113191247</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6736168665176964</v>
+        <v>0.6740255086446632</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7503719671250473</v>
+        <v>0.7506961663181104</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.829012261493037</v>
+        <v>1.827532081539733</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666376028037912</v>
+        <v>1.66442692177414</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.91418777953784</v>
+        <v>94.1628008016058</v>
       </c>
       <c r="D15" t="n">
-        <v>22.63935614324561</v>
+        <v>22.89926493004305</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -928,7 +928,7 @@
         <v>90.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>109.26</v>
+        <v>110.26</v>
       </c>
       <c r="I15" t="n">
         <v>145.26</v>
@@ -946,19 +946,19 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.80869979240862</v>
+        <v>-86.02480107908279</v>
       </c>
       <c r="D16" t="n">
-        <v>20.23570194439699</v>
+        <v>20.47195713110109</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.9574620641016</v>
+        <v>-102.7376019773414</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.0778545523916</v>
+        <v>-84.23249407632485</v>
       </c>
       <c r="H16" t="n">
         <v>-70.46683163887967</v>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.33885242742906</v>
+        <v>-78.60532520044909</v>
       </c>
       <c r="D17" t="n">
-        <v>25.18574384850274</v>
+        <v>25.44454038663521</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.2376019773414</v>
+        <v>-93.87736039420676</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.49305820175223</v>
+        <v>-73.57382219273629</v>
       </c>
       <c r="H17" t="n">
         <v>-60.41392685158225</v>

</xml_diff>